<commit_message>
Made Yeezus an instantiatable object, and separated it from Main, and.... did a lot of stuff
</commit_message>
<xml_diff>
--- a/Yeezus/output/data.xlsx
+++ b/Yeezus/output/data.xlsx
@@ -13,10 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Template" r:id="rId1" sheetId="1"/>
-    <sheet name="FCFS-1" r:id="rId6" sheetId="2"/>
-    <sheet name="FCFS-4" r:id="rId7" sheetId="3"/>
-    <sheet name="Priority-1" r:id="rId8" sheetId="4"/>
-    <sheet name="Priority-4" r:id="rId9" sheetId="5"/>
+    <sheet name="FCFS-0" r:id="rId6" sheetId="2"/>
+    <sheet name="FCFS-1" r:id="rId7" sheetId="3"/>
+    <sheet name="FCFS-4" r:id="rId8" sheetId="4"/>
+    <sheet name="Priority-0" r:id="rId9" sheetId="5"/>
+    <sheet name="Priority-1" r:id="rId10" sheetId="6"/>
+    <sheet name="Priority-4" r:id="rId11" sheetId="7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="11">
   <si>
     <t>Process ID:</t>
   </si>
@@ -812,10 +814,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>46.0</v>
+        <v>14.0</v>
       </c>
       <c r="C2" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
@@ -825,15 +827,6 @@
       </c>
       <c r="F2" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7.0</v>
       </c>
     </row>
     <row r="3">
@@ -841,10 +834,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>57.0</v>
+        <v>22.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -854,15 +847,6 @@
       </c>
       <c r="F3" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J3">
-        <f>AVERAGE($C$2:$C$31)</f>
       </c>
     </row>
     <row r="4">
@@ -870,7 +854,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>62.0</v>
+        <v>26.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -883,15 +867,6 @@
       </c>
       <c r="F4" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -899,10 +874,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>64.0</v>
+        <v>28.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
@@ -912,15 +887,6 @@
       </c>
       <c r="F5" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -928,10 +894,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>65.0</v>
+        <v>31.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
@@ -941,15 +907,6 @@
       </c>
       <c r="F6" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -957,10 +914,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>67.0</v>
+        <v>35.0</v>
       </c>
       <c r="C7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -970,15 +927,6 @@
       </c>
       <c r="F7" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -986,7 +934,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>70.0</v>
+        <v>36.0</v>
       </c>
       <c r="C8" t="n">
         <v>1.0</v>
@@ -999,15 +947,6 @@
       </c>
       <c r="F8" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1015,7 +954,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>71.0</v>
+        <v>38.0</v>
       </c>
       <c r="C9" t="n">
         <v>1.0</v>
@@ -1028,15 +967,6 @@
       </c>
       <c r="F9" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -1044,10 +974,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>72.0</v>
+        <v>39.0</v>
       </c>
       <c r="C10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
@@ -1057,15 +987,6 @@
       </c>
       <c r="F10" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -1073,10 +994,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>74.0</v>
+        <v>40.0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -1086,15 +1007,6 @@
       </c>
       <c r="F11" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -1102,10 +1014,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>76.0</v>
+        <v>42.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
@@ -1116,22 +1028,13 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>77.0</v>
+        <v>43.0</v>
       </c>
       <c r="C13" t="n">
         <v>1.0</v>
@@ -1144,15 +1047,6 @@
       </c>
       <c r="F13" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1160,10 +1054,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>79.0</v>
+        <v>44.0</v>
       </c>
       <c r="C14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
@@ -1173,15 +1067,6 @@
       </c>
       <c r="F14" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1189,10 +1074,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>81.0</v>
+        <v>45.0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
@@ -1202,15 +1087,6 @@
       </c>
       <c r="F15" t="n">
         <v>10.0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -1218,10 +1094,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>82.0</v>
+        <v>46.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
@@ -1231,15 +1107,6 @@
       </c>
       <c r="F16" t="n">
         <v>11.0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -1247,7 +1114,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>84.0</v>
+        <v>47.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -1260,15 +1127,6 @@
       </c>
       <c r="F17" t="n">
         <v>5.0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -1276,7 +1134,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>84.0</v>
+        <v>47.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -1289,15 +1147,6 @@
       </c>
       <c r="F18" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -1305,10 +1154,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>86.0</v>
+        <v>48.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -1325,10 +1174,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>87.0</v>
+        <v>49.0</v>
       </c>
       <c r="C20" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -1345,7 +1194,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>92.0</v>
+        <v>50.0</v>
       </c>
       <c r="C21" t="n">
         <v>1.0</v>
@@ -1365,10 +1214,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>94.0</v>
+        <v>52.0</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -1385,7 +1234,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>96.0</v>
+        <v>53.0</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -1405,10 +1254,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>97.0</v>
+        <v>54.0</v>
       </c>
       <c r="C24" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
@@ -1425,10 +1274,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>101.0</v>
+        <v>54.0</v>
       </c>
       <c r="C25" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
@@ -1445,7 +1294,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>103.0</v>
+        <v>55.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -1465,7 +1314,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>104.0</v>
+        <v>56.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -1485,10 +1334,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>104.0</v>
+        <v>56.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
@@ -1505,7 +1354,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>105.0</v>
+        <v>57.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -1525,7 +1374,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>107.0</v>
+        <v>59.0</v>
       </c>
       <c r="C30" t="n">
         <v>1.0</v>
@@ -1545,7 +1394,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>108.0</v>
+        <v>59.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -1644,7 +1493,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>48.0</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -1662,7 +1511,7 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>7.0</v>
+        <v>20.0</v>
       </c>
       <c r="J2" t="n">
         <v>2.0</v>
@@ -1673,7 +1522,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>49.0</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -1687,14 +1536,14 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
-      <c r="H3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1.0</v>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="J3">
+        <f>AVERAGE($C$2:$C$31)</f>
       </c>
     </row>
     <row r="4">
@@ -1702,10 +1551,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>2.0</v>
+        <v>51.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -1716,14 +1565,14 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
-      <c r="H4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.0</v>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -1731,10 +1580,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>2.0</v>
+        <v>51.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
@@ -1745,14 +1594,14 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
-      <c r="H5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -1760,10 +1609,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>3.0</v>
+        <v>52.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
@@ -1775,13 +1624,13 @@
         <v>12.0</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J6">
-        <f>AVERAGE($C$2:$C$31)</f>
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -1789,10 +1638,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>52.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -1818,10 +1667,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>53.0</v>
       </c>
       <c r="C8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
@@ -1847,7 +1696,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>54.0</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -1876,7 +1725,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>4.0</v>
+        <v>54.0</v>
       </c>
       <c r="C10" t="n">
         <v>1.0</v>
@@ -1905,10 +1754,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
+        <v>55.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -1934,10 +1783,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>4.0</v>
+        <v>56.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
@@ -1963,10 +1812,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>57.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
@@ -1992,7 +1841,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>5.0</v>
+        <v>58.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -2021,7 +1870,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>5.0</v>
+        <v>58.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -2050,10 +1899,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>5.0</v>
+        <v>58.0</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
@@ -2079,7 +1928,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>6.0</v>
+        <v>59.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -2108,10 +1957,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>6.0</v>
+        <v>59.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
@@ -2137,10 +1986,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>6.0</v>
+        <v>60.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -2150,15 +1999,6 @@
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -2166,10 +2006,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>6.0</v>
+        <v>61.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -2179,15 +2019,6 @@
       </c>
       <c r="F20" t="n">
         <v>10.0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -2195,10 +2026,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>7.0</v>
+        <v>61.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -2208,15 +2039,6 @@
       </c>
       <c r="F21" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -2224,10 +2046,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>7.0</v>
+        <v>62.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -2244,10 +2066,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>7.0</v>
+        <v>63.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
@@ -2264,7 +2086,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>7.0</v>
+        <v>64.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -2284,10 +2106,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>8.0</v>
+        <v>64.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
@@ -2304,7 +2126,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>8.0</v>
+        <v>65.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -2324,7 +2146,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>8.0</v>
+        <v>66.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -2344,7 +2166,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>9.0</v>
+        <v>66.0</v>
       </c>
       <c r="C28" t="n">
         <v>0.0</v>
@@ -2364,10 +2186,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>9.0</v>
+        <v>67.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
@@ -2384,7 +2206,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>9.0</v>
+        <v>67.0</v>
       </c>
       <c r="C30" t="n">
         <v>0.0</v>
@@ -2404,10 +2226,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>9.0</v>
+        <v>68.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
@@ -2503,7 +2325,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>22.0</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -2521,7 +2343,7 @@
         <v>0.0</v>
       </c>
       <c r="I2" t="n">
-        <v>25.0</v>
+        <v>5.0</v>
       </c>
       <c r="J2" t="n">
         <v>1.0</v>
@@ -2532,10 +2354,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>15.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -2546,14 +2368,14 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J3">
-        <f>AVERAGE($C$2:$C$31)</f>
+      <c r="H3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -2561,10 +2383,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -2575,14 +2397,14 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
+      <c r="H4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -2590,7 +2412,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -2604,14 +2426,14 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
+      <c r="H5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -2619,7 +2441,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>19.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -2634,13 +2456,13 @@
         <v>12.0</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="J6">
+        <f>AVERAGE($C$2:$C$31)</f>
       </c>
     </row>
     <row r="7">
@@ -2648,10 +2470,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -2677,7 +2499,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -2706,10 +2528,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
@@ -2735,7 +2557,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>23.0</v>
+        <v>2.0</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -2764,10 +2586,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -2793,7 +2615,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>20.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -2822,10 +2644,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
@@ -2851,10 +2673,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C14" t="n">
         <v>1.0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
@@ -2880,7 +2702,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>23.0</v>
+        <v>3.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -2909,7 +2731,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -2938,7 +2760,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -2967,10 +2789,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>16.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
@@ -2996,7 +2818,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -3009,6 +2831,15 @@
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -3016,7 +2847,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>25.0</v>
+        <v>4.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -3029,6 +2860,15 @@
       </c>
       <c r="F20" t="n">
         <v>10.0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -3036,7 +2876,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>24.0</v>
+        <v>4.0</v>
       </c>
       <c r="C21" t="n">
         <v>1.0</v>
@@ -3049,6 +2889,15 @@
       </c>
       <c r="F21" t="n">
         <v>12.0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -3056,10 +2905,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>17.0</v>
+        <v>4.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -3076,7 +2925,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C23" t="n">
         <v>0.0</v>
@@ -3096,7 +2945,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -3116,7 +2965,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="C25" t="n">
         <v>1.0</v>
@@ -3136,7 +2985,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -3156,7 +3005,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>18.0</v>
+        <v>5.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -3179,7 +3028,7 @@
         <v>5.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
@@ -3196,7 +3045,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>20.0</v>
+        <v>5.0</v>
       </c>
       <c r="C29" t="n">
         <v>0.0</v>
@@ -3216,10 +3065,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>26.0</v>
+        <v>6.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
@@ -3236,7 +3085,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -3335,10 +3184,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
@@ -3348,15 +3197,6 @@
       </c>
       <c r="F2" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -3364,10 +3204,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -3377,15 +3217,6 @@
       </c>
       <c r="F3" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -3393,10 +3224,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="C4" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -3406,15 +3237,6 @@
       </c>
       <c r="F4" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -3422,10 +3244,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="C5" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
@@ -3435,15 +3257,6 @@
       </c>
       <c r="F5" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -3454,7 +3267,7 @@
         <v>12.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
@@ -3464,15 +3277,6 @@
       </c>
       <c r="F6" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J6">
-        <f>AVERAGE($C$2:$C$31)</f>
       </c>
     </row>
     <row r="7">
@@ -3480,10 +3284,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -3493,15 +3297,6 @@
       </c>
       <c r="F7" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -3509,7 +3304,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -3522,15 +3317,6 @@
       </c>
       <c r="F8" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -3538,10 +3324,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
@@ -3551,15 +3337,6 @@
       </c>
       <c r="F9" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -3567,10 +3344,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
@@ -3580,15 +3357,6 @@
       </c>
       <c r="F10" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -3596,10 +3364,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -3609,15 +3377,6 @@
       </c>
       <c r="F11" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -3625,10 +3384,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
@@ -3639,25 +3398,16 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
@@ -3667,15 +3417,6 @@
       </c>
       <c r="F13" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -3686,7 +3427,7 @@
         <v>1.0</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
@@ -3696,15 +3437,6 @@
       </c>
       <c r="F14" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -3712,10 +3444,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
@@ -3725,15 +3457,6 @@
       </c>
       <c r="F15" t="n">
         <v>10.0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -3741,7 +3464,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -3754,15 +3477,6 @@
       </c>
       <c r="F16" t="n">
         <v>11.0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -3770,7 +3484,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -3783,15 +3497,6 @@
       </c>
       <c r="F17" t="n">
         <v>5.0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -3799,10 +3504,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
@@ -3812,15 +3517,6 @@
       </c>
       <c r="F18" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -3831,7 +3527,7 @@
         <v>1.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -3841,15 +3537,6 @@
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -3857,10 +3544,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -3870,15 +3557,6 @@
       </c>
       <c r="F20" t="n">
         <v>10.0</v>
-      </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -3886,10 +3564,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -3899,15 +3577,6 @@
       </c>
       <c r="F21" t="n">
         <v>12.0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -3918,7 +3587,7 @@
         <v>11.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -3938,7 +3607,7 @@
         <v>2.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
@@ -3955,7 +3624,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -3975,10 +3644,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C25" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
@@ -3995,7 +3664,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -4015,10 +3684,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
@@ -4035,10 +3704,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
@@ -4055,10 +3724,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
@@ -4075,10 +3744,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
@@ -4095,10 +3764,1701 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D31">
+        <f>$B$31+$C$31</f>
+      </c>
+      <c r="E31" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="C32">
+        <f>AVERAGE($C$2:$C$31)</f>
+      </c>
+      <c r="D32">
+        <f>AVERAGE($D$2:$D$31)</f>
+      </c>
+      <c r="E32">
+        <f>AVERAGE($E$2:$E$31)</f>
+      </c>
+      <c r="F32">
+        <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2">
+        <f>$B$2+$C$2</f>
+      </c>
+      <c r="E2" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3">
+        <f>$B$3+$C$3</f>
+      </c>
+      <c r="E3" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="J3">
+        <f>AVERAGE($C$2:$C$31)</f>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3.0</v>
       </c>
+      <c r="B4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4">
+        <f>$B$4+$C$4</f>
+      </c>
+      <c r="E4" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5">
+        <f>$B$5+$C$5</f>
+      </c>
+      <c r="E5" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6">
+        <f>$B$6+$C$6</f>
+      </c>
+      <c r="E6" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7">
+        <f>$B$7+$C$7</f>
+      </c>
+      <c r="E7" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8">
+        <f>$B$8+$C$8</f>
+      </c>
+      <c r="E8" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9">
+        <f>$B$9+$C$9</f>
+      </c>
+      <c r="E9" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10">
+        <f>$B$10+$C$10</f>
+      </c>
+      <c r="E10" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D11">
+        <f>$B$11+$C$11</f>
+      </c>
+      <c r="E11" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12">
+        <f>$B$12+$C$12</f>
+      </c>
+      <c r="E12" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D13">
+        <f>$B$13+$C$13</f>
+      </c>
+      <c r="E13" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D14">
+        <f>$B$14+$C$14</f>
+      </c>
+      <c r="E14" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15">
+        <f>$B$15+$C$15</f>
+      </c>
+      <c r="E15" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16">
+        <f>$B$16+$C$16</f>
+      </c>
+      <c r="E16" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17">
+        <f>$B$17+$C$17</f>
+      </c>
+      <c r="E17" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18">
+        <f>$B$18+$C$18</f>
+      </c>
+      <c r="E18" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D19">
+        <f>$B$19+$C$19</f>
+      </c>
+      <c r="E19" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D20">
+        <f>$B$20+$C$20</f>
+      </c>
+      <c r="E20" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D21">
+        <f>$B$21+$C$21</f>
+      </c>
+      <c r="E21" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D22">
+        <f>$B$22+$C$22</f>
+      </c>
+      <c r="E22" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D23">
+        <f>$B$23+$C$23</f>
+      </c>
+      <c r="E23" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D24">
+        <f>$B$24+$C$24</f>
+      </c>
+      <c r="E24" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25">
+        <f>$B$25+$C$25</f>
+      </c>
+      <c r="E25" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26">
+        <f>$B$26+$C$26</f>
+      </c>
+      <c r="E26" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D27">
+        <f>$B$27+$C$27</f>
+      </c>
+      <c r="E27" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28">
+        <f>$B$28+$C$28</f>
+      </c>
+      <c r="E28" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29">
+        <f>$B$29+$C$29</f>
+      </c>
+      <c r="E29" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D30">
+        <f>$B$30+$C$30</f>
+      </c>
+      <c r="E30" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>6.0</v>
+      </c>
       <c r="C31" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D31">
+        <f>$B$31+$C$31</f>
+      </c>
+      <c r="E31" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="C32">
+        <f>AVERAGE($C$2:$C$31)</f>
+      </c>
+      <c r="D32">
+        <f>AVERAGE($D$2:$D$31)</f>
+      </c>
+      <c r="E32">
+        <f>AVERAGE($E$2:$E$31)</f>
+      </c>
+      <c r="F32">
+        <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D2">
+        <f>$B$2+$C$2</f>
+      </c>
+      <c r="E2" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3">
+        <f>$B$3+$C$3</f>
+      </c>
+      <c r="E3" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4">
+        <f>$B$4+$C$4</f>
+      </c>
+      <c r="E4" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5">
+        <f>$B$5+$C$5</f>
+      </c>
+      <c r="E5" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D6">
+        <f>$B$6+$C$6</f>
+      </c>
+      <c r="E6" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f>AVERAGE($B$2:$B$31)</f>
+      </c>
+      <c r="J6">
+        <f>AVERAGE($C$2:$C$31)</f>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7">
+        <f>$B$7+$C$7</f>
+      </c>
+      <c r="E7" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8">
+        <f>$B$8+$C$8</f>
+      </c>
+      <c r="E8" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D9">
+        <f>$B$9+$C$9</f>
+      </c>
+      <c r="E9" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10">
+        <f>$B$10+$C$10</f>
+      </c>
+      <c r="E10" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D11">
+        <f>$B$11+$C$11</f>
+      </c>
+      <c r="E11" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D12">
+        <f>$B$12+$C$12</f>
+      </c>
+      <c r="E12" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D13">
+        <f>$B$13+$C$13</f>
+      </c>
+      <c r="E13" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14">
+        <f>$B$14+$C$14</f>
+      </c>
+      <c r="E14" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D15">
+        <f>$B$15+$C$15</f>
+      </c>
+      <c r="E15" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D16">
+        <f>$B$16+$C$16</f>
+      </c>
+      <c r="E16" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D17">
+        <f>$B$17+$C$17</f>
+      </c>
+      <c r="E17" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D18">
+        <f>$B$18+$C$18</f>
+      </c>
+      <c r="E18" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D19">
+        <f>$B$19+$C$19</f>
+      </c>
+      <c r="E19" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D20">
+        <f>$B$20+$C$20</f>
+      </c>
+      <c r="E20" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D21">
+        <f>$B$21+$C$21</f>
+      </c>
+      <c r="E21" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D22">
+        <f>$B$22+$C$22</f>
+      </c>
+      <c r="E22" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D23">
+        <f>$B$23+$C$23</f>
+      </c>
+      <c r="E23" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D24">
+        <f>$B$24+$C$24</f>
+      </c>
+      <c r="E24" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D25">
+        <f>$B$25+$C$25</f>
+      </c>
+      <c r="E25" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26">
+        <f>$B$26+$C$26</f>
+      </c>
+      <c r="E26" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D27">
+        <f>$B$27+$C$27</f>
+      </c>
+      <c r="E27" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D28">
+        <f>$B$28+$C$28</f>
+      </c>
+      <c r="E28" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D29">
+        <f>$B$29+$C$29</f>
+      </c>
+      <c r="E29" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D30">
+        <f>$B$30+$C$30</f>
+      </c>
+      <c r="E30" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>

</xml_diff>

<commit_message>
Outputted more Excel data
</commit_message>
<xml_diff>
--- a/Yeezus/output/data.xlsx
+++ b/Yeezus/output/data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="14">
   <si>
     <t>Process ID:</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Idle Time (ms):</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>% of RAM</t>
+  </si>
+  <si>
+    <t>% of Cache</t>
   </si>
   <si>
     <t/>
@@ -147,7 +156,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="Process_Table" id="1" name="Process_Table" ref="A1:F32" totalsRowCount="1">
   <autoFilter ref="A1:F32"/>
-  <tableColumns count="6">
+  <tableColumns count="9">
     <tableColumn id="1" name="Process ID:" totalsRowDxfId="0" totalsRowLabel="Average"/>
     <tableColumn id="2" name="Wait Time (ms):" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[Wait Time (ms):])</totalsRowFormula>
@@ -165,14 +174,21 @@
     <tableColumn id="6" name="I/O Count:" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Process_Table[I/O Count:])</totalsRowFormula>
     </tableColumn>
+    <tableColumn id="8" name="CPU"/>
+    <tableColumn id="9" name="% of Cache" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Process_Table[% of Cache])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="7" name="% of RAM" totalsRowFunction="custom">
+      <totalsRowFormula>AVERAGE(Process_Table[% of RAM])</totalsRowFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="CPU_Table" id="2" insertRow="1" name="CPU_Table" ref="H1:J6" totalsRowCount="1">
-  <autoFilter ref="H1:J6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="CPU_Table" id="2" insertRow="1" name="CPU_Table" ref="K1:M6" totalsRowCount="1">
+  <autoFilter ref="K1:M6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="CPU ID:" totalsRowLabel="Average"/>
     <tableColumn id="2" name="Busy Time (ms):" totalsRowFunction="custom">
@@ -483,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,13 +512,16 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,208 +540,217 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D3">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" t="e">
-        <f>AVERAGE(Template!I2:I2)</f>
+      <c r="L3" t="e">
+        <f>AVERAGE(Template!L2:L2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J3" t="e">
-        <f>AVERAGE(Template!J2:J2)</f>
+      <c r="M3" t="e">
+        <f>AVERAGE(Template!M2:M2)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D5">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D7">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D9">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D11">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D12">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D13">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D15">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D16">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D17">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D22">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D23">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D24">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D26">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D27">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31">
         <f>Template!C2:C31+Template!B2:B31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -744,6 +772,14 @@
       </c>
       <c r="F32" t="e">
         <f>AVERAGE(Template!F2:F31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" t="e">
+        <f>AVERAGE(Template!H2:H31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I32" t="e">
+        <f>AVERAGE(Template!I2:I31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -759,10 +795,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,13 +808,16 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,13 +836,22 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -812,10 +860,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>46.0</v>
+        <v>48.0</v>
       </c>
       <c r="C2" t="n">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
@@ -826,14 +874,23 @@
       <c r="F2" t="n">
         <v>12.0</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.67</v>
       </c>
       <c r="I2" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>7.0</v>
+        <v>0.0654296875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="3">
@@ -844,7 +901,7 @@
         <v>57.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -855,14 +912,23 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="I3">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J3">
-        <f>AVERAGE($C$2:$C$31)</f>
+      <c r="L3">
+        <f>AVERAGE($L$2:$L$2)</f>
+      </c>
+      <c r="M3">
+        <f>AVERAGE($M$2:$M$2)</f>
       </c>
     </row>
     <row r="4">
@@ -870,10 +936,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>62.0</v>
+        <v>60.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -884,14 +950,23 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -913,14 +988,23 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -928,7 +1012,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -942,14 +1026,23 @@
       <c r="F6" t="n">
         <v>12.0</v>
       </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -957,7 +1050,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>67.0</v>
+        <v>68.0</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
@@ -971,14 +1064,23 @@
       <c r="F7" t="n">
         <v>12.0</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -1000,14 +1102,23 @@
       <c r="F8" t="n">
         <v>12.0</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -1015,10 +1126,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>71.0</v>
+        <v>72.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
@@ -1029,14 +1140,23 @@
       <c r="F9" t="n">
         <v>12.0</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -1044,10 +1164,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>72.0</v>
+        <v>74.0</v>
       </c>
       <c r="C10" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
@@ -1058,14 +1178,23 @@
       <c r="F10" t="n">
         <v>12.0</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -1073,10 +1202,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>74.0</v>
+        <v>76.0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -1087,14 +1216,23 @@
       <c r="F11" t="n">
         <v>12.0</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -1102,10 +1240,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>76.0</v>
+        <v>79.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
@@ -1116,14 +1254,23 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -1131,10 +1278,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>77.0</v>
+        <v>82.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
@@ -1145,14 +1292,23 @@
       <c r="F13" t="n">
         <v>12.0</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1160,10 +1316,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>79.0</v>
+        <v>84.0</v>
       </c>
       <c r="C14" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
@@ -1174,14 +1330,23 @@
       <c r="F14" t="n">
         <v>12.0</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -1189,10 +1354,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>81.0</v>
+        <v>85.0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
@@ -1203,14 +1368,23 @@
       <c r="F15" t="n">
         <v>10.0</v>
       </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -1218,7 +1392,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>82.0</v>
+        <v>86.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -1232,14 +1406,23 @@
       <c r="F16" t="n">
         <v>11.0</v>
       </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -1247,7 +1430,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>84.0</v>
+        <v>87.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -1261,14 +1444,23 @@
       <c r="F17" t="n">
         <v>5.0</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
+      <c r="G17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -1276,7 +1468,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>84.0</v>
+        <v>88.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -1290,14 +1482,23 @@
       <c r="F18" t="n">
         <v>12.0</v>
       </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -1305,7 +1506,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>86.0</v>
+        <v>90.0</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
@@ -1318,6 +1519,15 @@
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="20">
@@ -1325,10 +1535,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>87.0</v>
+        <v>92.0</v>
       </c>
       <c r="C20" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -1338,6 +1548,15 @@
       </c>
       <c r="F20" t="n">
         <v>10.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="21">
@@ -1345,7 +1564,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>92.0</v>
+        <v>93.0</v>
       </c>
       <c r="C21" t="n">
         <v>1.0</v>
@@ -1358,6 +1577,15 @@
       </c>
       <c r="F21" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="22">
@@ -1365,10 +1593,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>94.0</v>
+        <v>95.0</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -1378,6 +1606,15 @@
       </c>
       <c r="F22" t="n">
         <v>13.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="23">
@@ -1388,7 +1625,7 @@
         <v>96.0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
@@ -1398,6 +1635,15 @@
       </c>
       <c r="F23" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="24">
@@ -1405,10 +1651,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>97.0</v>
+        <v>99.0</v>
       </c>
       <c r="C24" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
@@ -1418,6 +1664,15 @@
       </c>
       <c r="F24" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="25">
@@ -1425,7 +1680,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>101.0</v>
+        <v>100.0</v>
       </c>
       <c r="C25" t="n">
         <v>2.0</v>
@@ -1438,6 +1693,15 @@
       </c>
       <c r="F25" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="26">
@@ -1445,7 +1709,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>103.0</v>
+        <v>102.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -1458,6 +1722,15 @@
       </c>
       <c r="F26" t="n">
         <v>7.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="27">
@@ -1465,7 +1738,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>104.0</v>
+        <v>103.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -1478,6 +1751,15 @@
       </c>
       <c r="F27" t="n">
         <v>8.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="28">
@@ -1499,13 +1781,22 @@
       <c r="F28" t="n">
         <v>12.0</v>
       </c>
+      <c r="G28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0654296875</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>105.0</v>
+        <v>106.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -1518,6 +1809,15 @@
       </c>
       <c r="F29" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="30">
@@ -1539,6 +1839,15 @@
       <c r="F30" t="n">
         <v>12.0</v>
       </c>
+      <c r="G30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.06640625</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1559,6 +1868,15 @@
       <c r="F31" t="n">
         <v>11.0</v>
       </c>
+      <c r="G31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0615234375</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -1578,6 +1896,12 @@
       </c>
       <c r="F32">
         <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+      <c r="H32">
+        <f>AVERAGE($H$2:$H$31)</f>
+      </c>
+      <c r="I32">
+        <f>AVERAGE($I$2:$I$31)</f>
       </c>
     </row>
   </sheetData>
@@ -1591,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,13 +1928,16 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1629,13 +1956,22 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1658,13 +1994,22 @@
       <c r="F2" t="n">
         <v>12.0</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.67</v>
       </c>
       <c r="I2" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J2" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="M2" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -1676,7 +2021,7 @@
         <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -1687,14 +2032,23 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
+      <c r="G3" t="n">
+        <v>1.0</v>
+      </c>
       <c r="H3" t="n">
-        <v>1.0</v>
+        <v>0.72</v>
       </c>
       <c r="I3" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1.0</v>
+        <v>0.0703125</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -1705,7 +2059,7 @@
         <v>2.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -1716,14 +2070,23 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
+      <c r="G4" t="n">
+        <v>2.0</v>
+      </c>
       <c r="H4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K4" t="n">
         <v>2.0</v>
       </c>
-      <c r="I4" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.0</v>
+      <c r="L4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -1734,7 +2097,7 @@
         <v>2.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
@@ -1745,14 +2108,23 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
+      <c r="G5" t="n">
+        <v>3.0</v>
+      </c>
       <c r="H5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K5" t="n">
         <v>3.0</v>
       </c>
-      <c r="I5" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
+      <c r="L5" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -1774,14 +2146,23 @@
       <c r="F6" t="n">
         <v>12.0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="I6">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J6">
-        <f>AVERAGE($C$2:$C$31)</f>
+      <c r="L6">
+        <f>AVERAGE($L$2:$L$5)</f>
+      </c>
+      <c r="M6">
+        <f>AVERAGE($M$2:$M$5)</f>
       </c>
     </row>
     <row r="7">
@@ -1789,7 +2170,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C7" t="n">
         <v>1.0</v>
@@ -1803,14 +2184,23 @@
       <c r="F7" t="n">
         <v>12.0</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
+      <c r="G7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -1818,7 +2208,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C8" t="n">
         <v>1.0</v>
@@ -1832,14 +2222,23 @@
       <c r="F8" t="n">
         <v>12.0</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -1847,7 +2246,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="n">
         <v>0.0</v>
@@ -1861,14 +2260,23 @@
       <c r="F9" t="n">
         <v>12.0</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+      <c r="G9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -1876,7 +2284,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C10" t="n">
         <v>1.0</v>
@@ -1890,14 +2298,23 @@
       <c r="F10" t="n">
         <v>12.0</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -1905,7 +2322,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" t="n">
         <v>1.0</v>
@@ -1919,14 +2336,23 @@
       <c r="F11" t="n">
         <v>12.0</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
+      <c r="G11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -1934,10 +2360,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
@@ -1948,14 +2374,23 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -1963,7 +2398,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C13" t="n">
         <v>1.0</v>
@@ -1977,14 +2412,23 @@
       <c r="F13" t="n">
         <v>12.0</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
+      <c r="G13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -1992,7 +2436,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -2006,14 +2450,23 @@
       <c r="F14" t="n">
         <v>12.0</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
+      <c r="G14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -2021,7 +2474,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -2035,14 +2488,23 @@
       <c r="F15" t="n">
         <v>10.0</v>
       </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
+      <c r="G15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -2050,10 +2512,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
@@ -2064,14 +2526,23 @@
       <c r="F16" t="n">
         <v>11.0</v>
       </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -2079,7 +2550,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -2093,14 +2564,23 @@
       <c r="F17" t="n">
         <v>5.0</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
+      <c r="G17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -2108,7 +2588,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -2122,14 +2602,23 @@
       <c r="F18" t="n">
         <v>12.0</v>
       </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
+      <c r="G18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -2137,10 +2626,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -2151,14 +2640,23 @@
       <c r="F19" t="n">
         <v>12.0</v>
       </c>
-      <c r="H19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
+      <c r="G19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -2166,10 +2664,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -2180,14 +2678,23 @@
       <c r="F20" t="n">
         <v>10.0</v>
       </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
+      <c r="G20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -2209,14 +2716,23 @@
       <c r="F21" t="n">
         <v>12.0</v>
       </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>10</v>
+      <c r="G21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22">
@@ -2224,10 +2740,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -2237,6 +2753,15 @@
       </c>
       <c r="F22" t="n">
         <v>13.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="23">
@@ -2244,10 +2769,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
@@ -2257,6 +2782,15 @@
       </c>
       <c r="F23" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="24">
@@ -2264,10 +2798,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
@@ -2277,6 +2811,15 @@
       </c>
       <c r="F24" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="25">
@@ -2298,16 +2841,25 @@
       <c r="F25" t="n">
         <v>12.0</v>
       </c>
+      <c r="G25" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.06640625</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
@@ -2317,6 +2869,15 @@
       </c>
       <c r="F26" t="n">
         <v>7.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="27">
@@ -2324,7 +2885,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -2337,6 +2898,15 @@
       </c>
       <c r="F27" t="n">
         <v>8.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="28">
@@ -2358,6 +2928,15 @@
       <c r="F28" t="n">
         <v>12.0</v>
       </c>
+      <c r="G28" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0654296875</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2378,6 +2957,15 @@
       <c r="F29" t="n">
         <v>12.0</v>
       </c>
+      <c r="G29" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0703125</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2387,7 +2975,7 @@
         <v>9.0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
@@ -2397,6 +2985,15 @@
       </c>
       <c r="F30" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="31">
@@ -2418,6 +3015,15 @@
       <c r="F31" t="n">
         <v>11.0</v>
       </c>
+      <c r="G31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0615234375</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -2437,6 +3043,12 @@
       </c>
       <c r="F32">
         <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+      <c r="H32">
+        <f>AVERAGE($H$2:$H$31)</f>
+      </c>
+      <c r="I32">
+        <f>AVERAGE($I$2:$I$31)</f>
       </c>
     </row>
   </sheetData>
@@ -2450,10 +3062,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,13 +3075,16 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2488,13 +3103,22 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2503,7 +3127,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>22.0</v>
+        <v>19.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -2517,13 +3141,22 @@
       <c r="F2" t="n">
         <v>12.0</v>
       </c>
+      <c r="G2" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.67</v>
       </c>
       <c r="I2" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="J2" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="M2" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -2532,10 +3165,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -2546,14 +3179,23 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="I3">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J3">
-        <f>AVERAGE($C$2:$C$31)</f>
+      <c r="L3">
+        <f>AVERAGE($L$2:$L$2)</f>
+      </c>
+      <c r="M3">
+        <f>AVERAGE($M$2:$M$2)</f>
       </c>
     </row>
     <row r="4">
@@ -2564,7 +3206,7 @@
         <v>11.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -2575,14 +3217,23 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -2604,14 +3255,23 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -2619,7 +3279,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>19.0</v>
+        <v>16.0</v>
       </c>
       <c r="C6" t="n">
         <v>0.0</v>
@@ -2633,14 +3293,23 @@
       <c r="F6" t="n">
         <v>12.0</v>
       </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>10</v>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -2648,10 +3317,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -2662,14 +3331,23 @@
       <c r="F7" t="n">
         <v>12.0</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -2677,7 +3355,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C8" t="n">
         <v>0.0</v>
@@ -2691,14 +3369,23 @@
       <c r="F8" t="n">
         <v>12.0</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -2709,7 +3396,7 @@
         <v>0.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
@@ -2720,14 +3407,23 @@
       <c r="F9" t="n">
         <v>12.0</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -2735,7 +3431,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>23.0</v>
+        <v>19.0</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
@@ -2749,14 +3445,23 @@
       <c r="F10" t="n">
         <v>12.0</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -2764,7 +3469,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" t="n">
         <v>0.0</v>
@@ -2778,14 +3483,23 @@
       <c r="F11" t="n">
         <v>12.0</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -2793,7 +3507,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>20.0</v>
+        <v>17.0</v>
       </c>
       <c r="C12" t="n">
         <v>0.0</v>
@@ -2807,14 +3521,23 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -2822,7 +3545,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C13" t="n">
         <v>0.0</v>
@@ -2836,14 +3559,23 @@
       <c r="F13" t="n">
         <v>12.0</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -2851,7 +3583,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -2865,14 +3597,23 @@
       <c r="F14" t="n">
         <v>12.0</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -2880,7 +3621,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>23.0</v>
+        <v>20.0</v>
       </c>
       <c r="C15" t="n">
         <v>0.0</v>
@@ -2894,14 +3635,23 @@
       <c r="F15" t="n">
         <v>10.0</v>
       </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -2909,10 +3659,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
@@ -2923,14 +3673,23 @@
       <c r="F16" t="n">
         <v>11.0</v>
       </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -2938,7 +3697,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -2952,14 +3711,23 @@
       <c r="F17" t="n">
         <v>5.0</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
+      <c r="G17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -2967,10 +3735,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
@@ -2981,14 +3749,23 @@
       <c r="F18" t="n">
         <v>12.0</v>
       </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
+      <c r="G18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -2996,7 +3773,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -3009,6 +3786,15 @@
       </c>
       <c r="F19" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="20">
@@ -3016,7 +3802,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>25.0</v>
+        <v>21.0</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
@@ -3029,6 +3815,15 @@
       </c>
       <c r="F20" t="n">
         <v>10.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="21">
@@ -3036,10 +3831,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -3049,6 +3844,15 @@
       </c>
       <c r="F21" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="22">
@@ -3056,10 +3860,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>17.0</v>
+        <v>15.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -3069,6 +3873,15 @@
       </c>
       <c r="F22" t="n">
         <v>13.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="23">
@@ -3076,10 +3889,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C23" t="n">
         <v>3.0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
@@ -3089,6 +3902,15 @@
       </c>
       <c r="F23" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="24">
@@ -3096,7 +3918,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="C24" t="n">
         <v>0.0</v>
@@ -3109,6 +3931,15 @@
       </c>
       <c r="F24" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="25">
@@ -3116,10 +3947,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
@@ -3129,6 +3960,15 @@
       </c>
       <c r="F25" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="26">
@@ -3136,7 +3976,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -3149,6 +3989,15 @@
       </c>
       <c r="F26" t="n">
         <v>7.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="27">
@@ -3156,7 +4005,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="C27" t="n">
         <v>0.0</v>
@@ -3169,6 +4018,15 @@
       </c>
       <c r="F27" t="n">
         <v>8.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="28">
@@ -3176,10 +4034,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
@@ -3189,6 +4047,15 @@
       </c>
       <c r="F28" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="29">
@@ -3196,7 +4063,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>20.0</v>
+        <v>17.0</v>
       </c>
       <c r="C29" t="n">
         <v>0.0</v>
@@ -3209,6 +4076,15 @@
       </c>
       <c r="F29" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="30">
@@ -3216,10 +4092,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
@@ -3229,6 +4105,15 @@
       </c>
       <c r="F30" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="31">
@@ -3236,7 +4121,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -3249,6 +4134,15 @@
       </c>
       <c r="F31" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="32">
@@ -3269,6 +4163,12 @@
       </c>
       <c r="F32">
         <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+      <c r="H32">
+        <f>AVERAGE($H$2:$H$31)</f>
+      </c>
+      <c r="I32">
+        <f>AVERAGE($I$2:$I$31)</f>
       </c>
     </row>
   </sheetData>
@@ -3282,10 +4182,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3295,13 +4195,16 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3320,13 +4223,22 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
       <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3335,10 +4247,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
@@ -3349,13 +4261,22 @@
       <c r="F2" t="n">
         <v>12.0</v>
       </c>
+      <c r="G2" t="n">
+        <v>3.0</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.67</v>
       </c>
       <c r="I2" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J2" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="M2" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -3364,10 +4285,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -3378,14 +4299,23 @@
       <c r="F3" t="n">
         <v>12.0</v>
       </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H3" t="n">
-        <v>1.0</v>
+        <v>0.72</v>
       </c>
       <c r="I3" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3.0</v>
+        <v>0.0703125</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
@@ -3393,10 +4323,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C4" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
@@ -3407,13 +4337,22 @@
       <c r="F4" t="n">
         <v>12.0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
       <c r="H4" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K4" t="n">
         <v>2.0</v>
       </c>
-      <c r="I4" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="M4" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -3422,10 +4361,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C5" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
@@ -3436,14 +4375,23 @@
       <c r="F5" t="n">
         <v>12.0</v>
       </c>
+      <c r="G5" t="n">
+        <v>3.0</v>
+      </c>
       <c r="H5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K5" t="n">
         <v>3.0</v>
       </c>
-      <c r="I5" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3.0</v>
+      <c r="L5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -3451,7 +4399,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>12.0</v>
+        <v>9.0</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
@@ -3465,14 +4413,23 @@
       <c r="F6" t="n">
         <v>12.0</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K6" t="s">
         <v>4</v>
       </c>
-      <c r="I6">
-        <f>AVERAGE($B$2:$B$31)</f>
-      </c>
-      <c r="J6">
-        <f>AVERAGE($C$2:$C$31)</f>
+      <c r="L6">
+        <f>AVERAGE($L$2:$L$5)</f>
+      </c>
+      <c r="M6">
+        <f>AVERAGE($M$2:$M$5)</f>
       </c>
     </row>
     <row r="7">
@@ -3480,10 +4437,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -3494,14 +4451,23 @@
       <c r="F7" t="n">
         <v>12.0</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
+      <c r="G7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -3509,10 +4475,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
@@ -3523,14 +4489,23 @@
       <c r="F8" t="n">
         <v>12.0</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
+      <c r="G8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9">
@@ -3538,10 +4513,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
@@ -3552,14 +4527,23 @@
       <c r="F9" t="n">
         <v>12.0</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" t="s">
-        <v>10</v>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -3567,10 +4551,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
@@ -3581,14 +4565,23 @@
       <c r="F10" t="n">
         <v>12.0</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
+      <c r="G10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11">
@@ -3596,10 +4589,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
@@ -3610,14 +4603,23 @@
       <c r="F11" t="n">
         <v>12.0</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
+      <c r="G11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -3625,7 +4627,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>12.0</v>
+        <v>9.0</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
@@ -3639,14 +4641,23 @@
       <c r="F12" t="n">
         <v>12.0</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
+      <c r="G12" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0654296875</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -3654,10 +4665,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
@@ -3668,14 +4679,23 @@
       <c r="F13" t="n">
         <v>12.0</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
+      <c r="G13" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -3683,10 +4703,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
@@ -3697,14 +4717,23 @@
       <c r="F14" t="n">
         <v>12.0</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
+      <c r="G14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -3712,10 +4741,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
@@ -3726,14 +4755,23 @@
       <c r="F15" t="n">
         <v>10.0</v>
       </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -3741,7 +4779,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -3755,14 +4793,23 @@
       <c r="F16" t="n">
         <v>11.0</v>
       </c>
-      <c r="H16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>10</v>
+      <c r="G16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -3770,7 +4817,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -3784,14 +4831,23 @@
       <c r="F17" t="n">
         <v>5.0</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
+      <c r="G17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.0615234375</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -3799,7 +4855,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -3813,14 +4869,23 @@
       <c r="F18" t="n">
         <v>12.0</v>
       </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>10</v>
+      <c r="G18" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19">
@@ -3828,10 +4893,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -3842,14 +4907,23 @@
       <c r="F19" t="n">
         <v>12.0</v>
       </c>
-      <c r="H19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" t="s">
-        <v>10</v>
+      <c r="G19" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -3857,10 +4931,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
@@ -3871,14 +4945,23 @@
       <c r="F20" t="n">
         <v>10.0</v>
       </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
+      <c r="G20" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.0703125</v>
+      </c>
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21">
@@ -3886,10 +4969,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -3900,14 +4983,23 @@
       <c r="F21" t="n">
         <v>12.0</v>
       </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>10</v>
+      <c r="G21" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.06640625</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22">
@@ -3915,10 +5007,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
@@ -3928,6 +5020,15 @@
       </c>
       <c r="F22" t="n">
         <v>13.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="23">
@@ -3935,7 +5036,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C23" t="n">
         <v>1.0</v>
@@ -3948,6 +5049,15 @@
       </c>
       <c r="F23" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="24">
@@ -3955,10 +5065,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
@@ -3968,6 +5078,15 @@
       </c>
       <c r="F24" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="25">
@@ -3975,10 +5094,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C25" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
@@ -3988,6 +5107,15 @@
       </c>
       <c r="F25" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="26">
@@ -3995,7 +5123,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -4008,6 +5136,15 @@
       </c>
       <c r="F26" t="n">
         <v>7.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="27">
@@ -4015,10 +5152,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
@@ -4028,6 +5165,15 @@
       </c>
       <c r="F27" t="n">
         <v>8.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="28">
@@ -4035,10 +5181,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C28" t="n">
         <v>2.0</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
@@ -4048,6 +5194,15 @@
       </c>
       <c r="F28" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0654296875</v>
       </c>
     </row>
     <row r="29">
@@ -4055,7 +5210,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -4068,6 +5223,15 @@
       </c>
       <c r="F29" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0.0703125</v>
       </c>
     </row>
     <row r="30">
@@ -4075,10 +5239,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>14.0</v>
+        <v>11.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
@@ -4088,6 +5252,15 @@
       </c>
       <c r="F30" t="n">
         <v>12.0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.06640625</v>
       </c>
     </row>
     <row r="31">
@@ -4095,7 +5268,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
@@ -4108,6 +5281,15 @@
       </c>
       <c r="F31" t="n">
         <v>11.0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.0615234375</v>
       </c>
     </row>
     <row r="32">
@@ -4128,6 +5310,12 @@
       </c>
       <c r="F32">
         <f>AVERAGE($F$2:$F$31)</f>
+      </c>
+      <c r="H32">
+        <f>AVERAGE($H$2:$H$31)</f>
+      </c>
+      <c r="I32">
+        <f>AVERAGE($I$2:$I$31)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Phase 2 Report and added some bugs
</commit_message>
<xml_diff>
--- a/Yeezus/output/data.xlsx
+++ b/Yeezus/output/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37715" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40028" uniqueCount="391">
   <si>
     <t>Process ID:</t>
   </si>
@@ -1953,6 +1953,131 @@
   <si>
     <t xml:space="preserve">
 CPU: 0 received 1513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 570
+CPU: 1 received 343
+CPU: 2 received 260
+CPU: 3 received 195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 492
+CPU: 1 received 307
+CPU: 2 received 297
+CPU: 3 received 278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 600
+CPU: 1 received 338
+CPU: 2 received 252
+CPU: 3 received 203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 798
+CPU: 1 received 390
+CPU: 2 received 283
+CPU: 3 received 238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 656
+CPU: 1 received 399
+CPU: 2 received 325
+CPU: 3 received 230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 515
+CPU: 1 received 266
+CPU: 2 received 291
+CPU: 3 received 272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 462
+CPU: 1 received 483
+CPU: 2 received 415
+CPU: 3 received 203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 2060</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 821
+CPU: 1 received 494
+CPU: 2 received 501
+CPU: 3 received 370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 820
+CPU: 1 received 316
+CPU: 2 received 264
+CPU: 3 received 232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 652
+CPU: 1 received 403
+CPU: 2 received 292
+CPU: 3 received 250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 469
+CPU: 1 received 387
+CPU: 2 received 307
+CPU: 3 received 222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 925</t>
   </si>
 </sst>
 </file>
@@ -2743,10 +2868,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="C2" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
@@ -2770,13 +2895,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>80.0</v>
+        <v>69.0</v>
       </c>
       <c r="M2" t="n">
-        <v>42.0</v>
+        <v>38.0</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3">
@@ -2784,10 +2909,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="C3" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
@@ -2822,19 +2947,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>43.0</v>
+        <v>45.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.0</v>
+        <v>13.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>141.0</v>
+        <v>147.0</v>
       </c>
       <c r="F4" t="n">
-        <v>12.0</v>
+        <v>18.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -2860,19 +2985,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>48.0</v>
+        <v>58.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>102.0</v>
+        <v>93.0</v>
       </c>
       <c r="F5" t="n">
-        <v>23.0</v>
+        <v>14.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -2898,19 +3023,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>51.0</v>
+        <v>62.0</v>
       </c>
       <c r="C6" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>167.0</v>
+        <v>151.0</v>
       </c>
       <c r="F6" t="n">
-        <v>28.0</v>
+        <v>12.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -2936,10 +3061,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>57.0</v>
+        <v>63.0</v>
       </c>
       <c r="C7" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
@@ -2974,7 +3099,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>60.0</v>
+        <v>68.0</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -2983,10 +3108,10 @@
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>137.0</v>
+        <v>146.0</v>
       </c>
       <c r="F8" t="n">
-        <v>58.0</v>
+        <v>67.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -3012,19 +3137,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>64.0</v>
+        <v>71.0</v>
       </c>
       <c r="C9" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>154.0</v>
+        <v>103.0</v>
       </c>
       <c r="F9" t="n">
-        <v>75.0</v>
+        <v>24.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -3050,7 +3175,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>67.0</v>
+        <v>72.0</v>
       </c>
       <c r="C10" t="n">
         <v>1.0</v>
@@ -3059,10 +3184,10 @@
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>145.0</v>
+        <v>146.0</v>
       </c>
       <c r="F10" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -3088,19 +3213,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>70.0</v>
+        <v>75.0</v>
       </c>
       <c r="C11" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>174.0</v>
+        <v>152.0</v>
       </c>
       <c r="F11" t="n">
-        <v>35.0</v>
+        <v>13.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -3126,19 +3251,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>81.0</v>
+        <v>77.0</v>
       </c>
       <c r="C12" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>142.0</v>
+        <v>140.0</v>
       </c>
       <c r="F12" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -3164,7 +3289,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>88.0</v>
+        <v>78.0</v>
       </c>
       <c r="C13" t="n">
         <v>2.0</v>
@@ -3173,10 +3298,10 @@
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>157.0</v>
+        <v>156.0</v>
       </c>
       <c r="F13" t="n">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -3202,7 +3327,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>90.0</v>
+        <v>81.0</v>
       </c>
       <c r="C14" t="n">
         <v>2.0</v>
@@ -3211,10 +3336,10 @@
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>141.0</v>
+        <v>143.0</v>
       </c>
       <c r="F14" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -3240,19 +3365,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>93.0</v>
+        <v>84.0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>111.0</v>
+        <v>143.0</v>
       </c>
       <c r="F15" t="n">
-        <v>46.0</v>
+        <v>78.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -3278,7 +3403,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>95.0</v>
+        <v>86.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -3316,19 +3441,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>97.0</v>
+        <v>87.0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>41.0</v>
+        <v>43.0</v>
       </c>
       <c r="F17" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -3354,19 +3479,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>99.0</v>
+        <v>89.0</v>
       </c>
       <c r="C18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>154.0</v>
+        <v>162.0</v>
       </c>
       <c r="F18" t="n">
-        <v>12.0</v>
+        <v>20.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -3392,10 +3517,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>101.0</v>
+        <v>92.0</v>
       </c>
       <c r="C19" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
@@ -3421,7 +3546,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>106.0</v>
+        <v>95.0</v>
       </c>
       <c r="C20" t="n">
         <v>1.0</v>
@@ -3430,10 +3555,10 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>121.0</v>
+        <v>124.0</v>
       </c>
       <c r="F20" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -3450,10 +3575,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>108.0</v>
+        <v>96.0</v>
       </c>
       <c r="C21" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -3479,19 +3604,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>114.0</v>
+        <v>99.0</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>111.0</v>
+        <v>168.0</v>
       </c>
       <c r="F22" t="n">
-        <v>25.0</v>
+        <v>82.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -3508,7 +3633,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>116.0</v>
+        <v>103.0</v>
       </c>
       <c r="C23" t="n">
         <v>1.0</v>
@@ -3517,10 +3642,10 @@
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>152.0</v>
+        <v>160.0</v>
       </c>
       <c r="F23" t="n">
-        <v>13.0</v>
+        <v>21.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -3537,7 +3662,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>118.0</v>
+        <v>105.0</v>
       </c>
       <c r="C24" t="n">
         <v>1.0</v>
@@ -3546,10 +3671,10 @@
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>127.0</v>
+        <v>130.0</v>
       </c>
       <c r="F24" t="n">
-        <v>11.0</v>
+        <v>14.0</v>
       </c>
       <c r="G24" t="n">
         <v>0.0</v>
@@ -3566,19 +3691,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>120.0</v>
+        <v>106.0</v>
       </c>
       <c r="C25" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>141.0</v>
+        <v>142.0</v>
       </c>
       <c r="F25" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -3595,7 +3720,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>123.0</v>
+        <v>108.0</v>
       </c>
       <c r="C26" t="n">
         <v>0.0</v>
@@ -3604,10 +3729,10 @@
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>75.0</v>
+        <v>82.0</v>
       </c>
       <c r="F26" t="n">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -3624,19 +3749,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>124.0</v>
+        <v>109.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>76.0</v>
+        <v>123.0</v>
       </c>
       <c r="F27" t="n">
-        <v>25.0</v>
+        <v>72.0</v>
       </c>
       <c r="G27" t="n">
         <v>0.0</v>
@@ -3653,7 +3778,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>126.0</v>
+        <v>112.0</v>
       </c>
       <c r="C28" t="n">
         <v>1.0</v>
@@ -3662,10 +3787,10 @@
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>140.0</v>
+        <v>143.0</v>
       </c>
       <c r="F28" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -3682,19 +3807,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>128.0</v>
+        <v>113.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>152.0</v>
+        <v>168.0</v>
       </c>
       <c r="F29" t="n">
-        <v>12.0</v>
+        <v>28.0</v>
       </c>
       <c r="G29" t="n">
         <v>0.0</v>
@@ -3711,7 +3836,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>129.0</v>
+        <v>115.0</v>
       </c>
       <c r="C30" t="n">
         <v>1.0</v>
@@ -3740,7 +3865,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>131.0</v>
+        <v>117.0</v>
       </c>
       <c r="C31" t="n">
         <v>1.0</v>
@@ -3749,10 +3874,10 @@
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>129.0</v>
+        <v>116.0</v>
       </c>
       <c r="F31" t="n">
-        <v>57.0</v>
+        <v>44.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -3866,16 +3991,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>277.0</v>
+        <v>207.0</v>
       </c>
       <c r="F2" t="n">
         <v>28.0</v>
@@ -3896,10 +4021,10 @@
         <v>23.0</v>
       </c>
       <c r="M2" t="n">
-        <v>21.0</v>
+        <v>29.0</v>
       </c>
       <c r="N2" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="3">
@@ -3907,22 +4032,22 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>163.0</v>
+        <v>170.0</v>
       </c>
       <c r="F3" t="n">
-        <v>19.0</v>
+        <v>16.0</v>
       </c>
       <c r="G3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n">
         <v>3.6</v>
@@ -3934,13 +4059,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="M3" t="n">
-        <v>26.0</v>
+        <v>35.0</v>
       </c>
       <c r="N3" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4">
@@ -3948,7 +4073,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -3957,13 +4082,13 @@
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>156.0</v>
+        <v>150.0</v>
       </c>
       <c r="F4" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.4</v>
@@ -3975,13 +4100,13 @@
         <v>2.0</v>
       </c>
       <c r="L4" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="M4" t="n">
-        <v>31.0</v>
+        <v>37.0</v>
       </c>
       <c r="N4" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5">
@@ -3989,22 +4114,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>163.0</v>
+        <v>85.0</v>
       </c>
       <c r="F5" t="n">
-        <v>70.0</v>
+        <v>40.0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H5" t="n">
         <v>3.15</v>
@@ -4016,13 +4141,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>16.0</v>
+        <v>10.0</v>
       </c>
       <c r="M5" t="n">
-        <v>27.0</v>
+        <v>43.0</v>
       </c>
       <c r="N5" t="s">
-        <v>366</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6">
@@ -4030,22 +4155,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>213.0</v>
+        <v>166.0</v>
       </c>
       <c r="F6" t="n">
-        <v>44.0</v>
+        <v>15.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H6" t="n">
         <v>3.6</v>
@@ -4068,22 +4193,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>11.0</v>
+        <v>7.0</v>
       </c>
       <c r="C7" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>372.0</v>
+        <v>173.0</v>
       </c>
       <c r="F7" t="n">
-        <v>111.0</v>
+        <v>20.0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H7" t="n">
         <v>3.4</v>
@@ -4106,22 +4231,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>117.0</v>
+        <v>258.0</v>
       </c>
       <c r="F8" t="n">
-        <v>48.0</v>
+        <v>107.0</v>
       </c>
       <c r="G8" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -4144,19 +4269,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>15.0</v>
+        <v>10.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>180.0</v>
+        <v>151.0</v>
       </c>
       <c r="F9" t="n">
-        <v>74.0</v>
+        <v>64.0</v>
       </c>
       <c r="G9" t="n">
         <v>3.0</v>
@@ -4182,22 +4307,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>17.0</v>
+        <v>11.0</v>
       </c>
       <c r="C10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>236.0</v>
+        <v>151.0</v>
       </c>
       <c r="F10" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="G10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H10" t="n">
         <v>3.4</v>
@@ -4220,22 +4345,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>17.0</v>
+        <v>14.0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>311.0</v>
+        <v>151.0</v>
       </c>
       <c r="F11" t="n">
-        <v>22.0</v>
+        <v>12.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H11" t="n">
         <v>3.6</v>
@@ -4258,7 +4383,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="C12" t="n">
         <v>2.0</v>
@@ -4267,10 +4392,10 @@
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>146.0</v>
+        <v>177.0</v>
       </c>
       <c r="F12" t="n">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -4296,22 +4421,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>59.0</v>
+        <v>185.0</v>
       </c>
       <c r="F13" t="n">
-        <v>4.0</v>
+        <v>18.0</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H13" t="n">
         <v>3.6</v>
@@ -4334,22 +4459,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>20.0</v>
+        <v>15.0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>134.0</v>
+        <v>142.0</v>
       </c>
       <c r="F14" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -4372,7 +4497,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>20.0</v>
+        <v>18.0</v>
       </c>
       <c r="C15" t="n">
         <v>1.0</v>
@@ -4381,13 +4506,13 @@
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>131.0</v>
+        <v>133.0</v>
       </c>
       <c r="F15" t="n">
-        <v>50.0</v>
+        <v>70.0</v>
       </c>
       <c r="G15" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H15" t="n">
         <v>3.15</v>
@@ -4410,7 +4535,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -4419,13 +4544,13 @@
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>144.0</v>
+        <v>128.0</v>
       </c>
       <c r="F16" t="n">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="G16" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H16" t="n">
         <v>3.4</v>
@@ -4448,19 +4573,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>23.0</v>
+        <v>20.0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>56.0</v>
+        <v>85.0</v>
       </c>
       <c r="F17" t="n">
-        <v>19.0</v>
+        <v>42.0</v>
       </c>
       <c r="G17" t="n">
         <v>3.0</v>
@@ -4486,22 +4611,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>23.0</v>
+        <v>21.0</v>
       </c>
       <c r="C18" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>188.0</v>
+        <v>161.0</v>
       </c>
       <c r="F18" t="n">
         <v>19.0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H18" t="n">
         <v>3.6</v>
@@ -4524,19 +4649,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>24.0</v>
+        <v>21.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>150.0</v>
+        <v>327.0</v>
       </c>
       <c r="F19" t="n">
-        <v>15.0</v>
+        <v>31.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -4571,13 +4696,13 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>188.0</v>
+        <v>209.0</v>
       </c>
       <c r="F20" t="n">
-        <v>16.0</v>
+        <v>28.0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H20" t="n">
         <v>3.6</v>
@@ -4600,22 +4725,22 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>153.0</v>
+        <v>238.0</v>
       </c>
       <c r="F21" t="n">
-        <v>14.0</v>
+        <v>49.0</v>
       </c>
       <c r="G21" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" t="n">
         <v>3.4</v>
@@ -4641,19 +4766,19 @@
         <v>27.0</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>314.0</v>
+        <v>338.0</v>
       </c>
       <c r="F22" t="n">
-        <v>112.0</v>
+        <v>252.0</v>
       </c>
       <c r="G22" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H22" t="n">
         <v>3.15</v>
@@ -4667,19 +4792,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>29.0</v>
+        <v>33.0</v>
       </c>
       <c r="C23" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>260.0</v>
+        <v>191.0</v>
       </c>
       <c r="F23" t="n">
-        <v>15.0</v>
+        <v>37.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -4696,7 +4821,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>36.0</v>
+        <v>34.0</v>
       </c>
       <c r="C24" t="n">
         <v>2.0</v>
@@ -4705,13 +4830,13 @@
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>198.0</v>
+        <v>260.0</v>
       </c>
       <c r="F24" t="n">
-        <v>23.0</v>
+        <v>43.0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -4725,22 +4850,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>38.0</v>
+        <v>35.0</v>
       </c>
       <c r="C25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>261.0</v>
+        <v>223.0</v>
       </c>
       <c r="F25" t="n">
-        <v>21.0</v>
+        <v>18.0</v>
       </c>
       <c r="G25" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H25" t="n">
         <v>3.4</v>
@@ -4754,7 +4879,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>38.0</v>
+        <v>36.0</v>
       </c>
       <c r="C26" t="n">
         <v>1.0</v>
@@ -4763,10 +4888,10 @@
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>84.0</v>
+        <v>95.0</v>
       </c>
       <c r="F26" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="G26" t="n">
         <v>1.0</v>
@@ -4783,19 +4908,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>58.0</v>
+        <v>205.0</v>
       </c>
       <c r="F27" t="n">
-        <v>22.0</v>
+        <v>134.0</v>
       </c>
       <c r="G27" t="n">
         <v>2.0</v>
@@ -4812,7 +4937,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>40.0</v>
+        <v>41.0</v>
       </c>
       <c r="C28" t="n">
         <v>1.0</v>
@@ -4821,13 +4946,13 @@
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>226.0</v>
+        <v>230.0</v>
       </c>
       <c r="F28" t="n">
-        <v>18.0</v>
+        <v>29.0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -4841,7 +4966,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>41.0</v>
+        <v>42.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -4850,13 +4975,13 @@
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>183.0</v>
+        <v>107.0</v>
       </c>
       <c r="F29" t="n">
-        <v>16.0</v>
+        <v>10.0</v>
       </c>
       <c r="G29" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H29" t="n">
         <v>3.6</v>
@@ -4870,22 +4995,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>42.0</v>
+        <v>43.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>223.0</v>
+        <v>355.0</v>
       </c>
       <c r="F30" t="n">
-        <v>16.0</v>
+        <v>32.0</v>
       </c>
       <c r="G30" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H30" t="n">
         <v>3.4</v>
@@ -4899,22 +5024,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>43.0</v>
+        <v>50.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>183.0</v>
+        <v>318.0</v>
       </c>
       <c r="F31" t="n">
-        <v>83.0</v>
+        <v>191.0</v>
       </c>
       <c r="G31" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>
@@ -5025,7 +5150,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>78.0</v>
+        <v>51.0</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -5034,10 +5159,10 @@
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>144.0</v>
+        <v>143.0</v>
       </c>
       <c r="F2" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -5052,13 +5177,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>54.0</v>
+        <v>47.0</v>
       </c>
       <c r="M2" t="n">
-        <v>32.0</v>
+        <v>16.0</v>
       </c>
       <c r="N2" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3">
@@ -5066,7 +5191,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>55.0</v>
+        <v>33.0</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -5075,10 +5200,10 @@
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>151.0</v>
+        <v>172.0</v>
       </c>
       <c r="F3" t="n">
-        <v>12.0</v>
+        <v>33.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -5104,19 +5229,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>37.0</v>
+        <v>20.0</v>
       </c>
       <c r="C4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>171.0</v>
+        <v>143.0</v>
       </c>
       <c r="F4" t="n">
-        <v>42.0</v>
+        <v>14.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -5142,19 +5267,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>46.0</v>
+        <v>24.0</v>
       </c>
       <c r="C5" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>215.0</v>
+        <v>137.0</v>
       </c>
       <c r="F5" t="n">
-        <v>136.0</v>
+        <v>58.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -5180,7 +5305,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>73.0</v>
+        <v>45.0</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -5189,10 +5314,10 @@
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>160.0</v>
+        <v>161.0</v>
       </c>
       <c r="F6" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -5218,7 +5343,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>33.0</v>
+        <v>18.0</v>
       </c>
       <c r="C7" t="n">
         <v>1.0</v>
@@ -5227,10 +5352,10 @@
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>145.0</v>
+        <v>158.0</v>
       </c>
       <c r="F7" t="n">
-        <v>16.0</v>
+        <v>29.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -5256,19 +5381,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>45.0</v>
+        <v>27.0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>203.0</v>
+        <v>166.0</v>
       </c>
       <c r="F8" t="n">
-        <v>124.0</v>
+        <v>87.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -5297,16 +5422,16 @@
         <v>1.0</v>
       </c>
       <c r="C9" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>213.0</v>
+        <v>145.0</v>
       </c>
       <c r="F9" t="n">
-        <v>134.0</v>
+        <v>66.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -5332,19 +5457,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>79.0</v>
+        <v>52.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>144.0</v>
+        <v>167.0</v>
       </c>
       <c r="F10" t="n">
-        <v>15.0</v>
+        <v>38.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -5370,7 +5495,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="C11" t="n">
         <v>1.0</v>
@@ -5379,10 +5504,10 @@
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>166.0</v>
+        <v>153.0</v>
       </c>
       <c r="F11" t="n">
-        <v>27.0</v>
+        <v>14.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -5408,7 +5533,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>74.0</v>
+        <v>45.0</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
@@ -5417,10 +5542,10 @@
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>158.0</v>
+        <v>140.0</v>
       </c>
       <c r="F12" t="n">
-        <v>30.0</v>
+        <v>12.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -5446,19 +5571,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>17.0</v>
+        <v>11.0</v>
       </c>
       <c r="C13" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>164.0</v>
+        <v>160.0</v>
       </c>
       <c r="F13" t="n">
-        <v>24.0</v>
+        <v>20.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -5484,7 +5609,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="C14" t="n">
         <v>1.0</v>
@@ -5493,10 +5618,10 @@
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>145.0</v>
+        <v>141.0</v>
       </c>
       <c r="F14" t="n">
-        <v>16.0</v>
+        <v>12.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -5522,19 +5647,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>82.0</v>
+        <v>55.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
       <c r="F15" t="n">
-        <v>45.0</v>
+        <v>35.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -5560,7 +5685,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>50.0</v>
+        <v>26.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -5598,19 +5723,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>27.0</v>
+        <v>15.0</v>
       </c>
       <c r="C17" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>125.0</v>
+        <v>46.0</v>
       </c>
       <c r="F17" t="n">
-        <v>95.0</v>
+        <v>16.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -5636,19 +5761,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>55.0</v>
+        <v>33.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>155.0</v>
+        <v>181.0</v>
       </c>
       <c r="F18" t="n">
-        <v>13.0</v>
+        <v>39.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -5674,7 +5799,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
@@ -5683,10 +5808,10 @@
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>153.0</v>
+        <v>142.0</v>
       </c>
       <c r="F19" t="n">
-        <v>24.0</v>
+        <v>13.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -5703,7 +5828,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>85.0</v>
+        <v>63.0</v>
       </c>
       <c r="C20" t="n">
         <v>1.0</v>
@@ -5712,10 +5837,10 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>121.0</v>
+        <v>132.0</v>
       </c>
       <c r="F20" t="n">
-        <v>10.0</v>
+        <v>21.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -5732,7 +5857,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>81.0</v>
+        <v>59.0</v>
       </c>
       <c r="C21" t="n">
         <v>1.0</v>
@@ -5741,10 +5866,10 @@
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>147.0</v>
+        <v>143.0</v>
       </c>
       <c r="F21" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -5761,19 +5886,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>66.0</v>
+        <v>38.0</v>
       </c>
       <c r="C22" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>170.0</v>
+        <v>162.0</v>
       </c>
       <c r="F22" t="n">
-        <v>84.0</v>
+        <v>76.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -5790,19 +5915,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>12.0</v>
+        <v>8.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>154.0</v>
+        <v>151.0</v>
       </c>
       <c r="F23" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -5819,7 +5944,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>51.0</v>
+        <v>28.0</v>
       </c>
       <c r="C24" t="n">
         <v>1.0</v>
@@ -5848,19 +5973,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>33.0</v>
+        <v>18.0</v>
       </c>
       <c r="C25" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>156.0</v>
+        <v>150.0</v>
       </c>
       <c r="F25" t="n">
-        <v>27.0</v>
+        <v>21.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -5877,19 +6002,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>16.0</v>
+        <v>11.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>92.0</v>
+        <v>76.0</v>
       </c>
       <c r="F26" t="n">
-        <v>24.0</v>
+        <v>8.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -5906,19 +6031,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>60.0</v>
+        <v>37.0</v>
       </c>
       <c r="C27" t="n">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>105.0</v>
+        <v>100.0</v>
       </c>
       <c r="F27" t="n">
-        <v>54.0</v>
+        <v>49.0</v>
       </c>
       <c r="G27" t="n">
         <v>0.0</v>
@@ -5935,19 +6060,19 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>19.0</v>
+        <v>12.0</v>
       </c>
       <c r="C28" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>202.0</v>
+        <v>164.0</v>
       </c>
       <c r="F28" t="n">
-        <v>74.0</v>
+        <v>36.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -5964,7 +6089,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>75.0</v>
+        <v>46.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -5993,7 +6118,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>85.0</v>
+        <v>63.0</v>
       </c>
       <c r="C30" t="n">
         <v>1.0</v>
@@ -6002,10 +6127,10 @@
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>157.0</v>
+        <v>164.0</v>
       </c>
       <c r="F30" t="n">
-        <v>28.0</v>
+        <v>35.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -6022,19 +6147,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="C31" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>221.0</v>
+        <v>108.0</v>
       </c>
       <c r="F31" t="n">
-        <v>149.0</v>
+        <v>36.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -6148,22 +6273,22 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>31.0</v>
+        <v>44.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>141.0</v>
+        <v>156.0</v>
       </c>
       <c r="F2" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="G2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H2" t="n">
         <v>3.35</v>
@@ -6175,13 +6300,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>14.0</v>
+        <v>22.0</v>
       </c>
       <c r="M2" t="n">
-        <v>21.0</v>
+        <v>25.0</v>
       </c>
       <c r="N2" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3">
@@ -6189,7 +6314,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>21.0</v>
+        <v>29.0</v>
       </c>
       <c r="C3" t="n">
         <v>2.0</v>
@@ -6198,13 +6323,13 @@
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>209.0</v>
+        <v>158.0</v>
       </c>
       <c r="F3" t="n">
-        <v>33.0</v>
+        <v>19.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H3" t="n">
         <v>3.6</v>
@@ -6216,13 +6341,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>12.0</v>
+        <v>22.0</v>
       </c>
       <c r="M3" t="n">
-        <v>22.0</v>
+        <v>25.0</v>
       </c>
       <c r="N3" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4">
@@ -6230,22 +6355,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>162.0</v>
+        <v>194.0</v>
       </c>
       <c r="F4" t="n">
-        <v>21.0</v>
+        <v>13.0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.4</v>
@@ -6257,13 +6382,13 @@
         <v>2.0</v>
       </c>
       <c r="L4" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="M4" t="n">
-        <v>24.0</v>
+        <v>36.0</v>
       </c>
       <c r="N4" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5">
@@ -6271,22 +6396,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>41.0</v>
+        <v>329.0</v>
       </c>
       <c r="F5" t="n">
-        <v>19.0</v>
+        <v>129.0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H5" t="n">
         <v>3.15</v>
@@ -6298,13 +6423,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="M5" t="n">
-        <v>26.0</v>
+        <v>37.0</v>
       </c>
       <c r="N5" t="s">
-        <v>364</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6">
@@ -6312,7 +6437,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>28.0</v>
+        <v>36.0</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -6321,13 +6446,13 @@
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>151.0</v>
+        <v>156.0</v>
       </c>
       <c r="F6" t="n">
-        <v>12.0</v>
+        <v>18.0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H6" t="n">
         <v>3.6</v>
@@ -6350,22 +6475,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>178.0</v>
+        <v>148.0</v>
       </c>
       <c r="F7" t="n">
-        <v>18.0</v>
+        <v>13.0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
         <v>3.4</v>
@@ -6388,22 +6513,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>16.0</v>
+        <v>22.0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>328.0</v>
+        <v>123.0</v>
       </c>
       <c r="F8" t="n">
-        <v>135.0</v>
+        <v>66.0</v>
       </c>
       <c r="G8" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -6429,19 +6554,19 @@
         <v>2.0</v>
       </c>
       <c r="C9" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>403.0</v>
+        <v>273.0</v>
       </c>
       <c r="F9" t="n">
-        <v>213.0</v>
+        <v>130.0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
         <v>3.15</v>
@@ -6464,19 +6589,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>31.0</v>
+        <v>44.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>152.0</v>
+        <v>157.0</v>
       </c>
       <c r="F10" t="n">
-        <v>18.0</v>
+        <v>28.0</v>
       </c>
       <c r="G10" t="n">
         <v>1.0</v>
@@ -6502,19 +6627,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>166.0</v>
+        <v>277.0</v>
       </c>
       <c r="F11" t="n">
-        <v>15.0</v>
+        <v>24.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -6540,7 +6665,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>28.0</v>
+        <v>36.0</v>
       </c>
       <c r="C12" t="n">
         <v>3.0</v>
@@ -6549,13 +6674,13 @@
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>141.0</v>
+        <v>262.0</v>
       </c>
       <c r="F12" t="n">
-        <v>13.0</v>
+        <v>22.0</v>
       </c>
       <c r="G12" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
         <v>3.35</v>
@@ -6581,16 +6706,16 @@
         <v>8.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>163.0</v>
+        <v>276.0</v>
       </c>
       <c r="F13" t="n">
-        <v>15.0</v>
+        <v>51.0</v>
       </c>
       <c r="G13" t="n">
         <v>2.0</v>
@@ -6616,7 +6741,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C14" t="n">
         <v>1.0</v>
@@ -6625,13 +6750,13 @@
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>142.0</v>
+        <v>219.0</v>
       </c>
       <c r="F14" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="G14" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -6654,19 +6779,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>31.0</v>
+        <v>41.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>249.0</v>
+        <v>486.0</v>
       </c>
       <c r="F15" t="n">
-        <v>85.0</v>
+        <v>261.0</v>
       </c>
       <c r="G15" t="n">
         <v>2.0</v>
@@ -6692,19 +6817,19 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>15.0</v>
+        <v>20.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>207.0</v>
+        <v>128.0</v>
       </c>
       <c r="F16" t="n">
-        <v>19.0</v>
+        <v>11.0</v>
       </c>
       <c r="G16" t="n">
         <v>0.0</v>
@@ -6730,7 +6855,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="C17" t="n">
         <v>1.0</v>
@@ -6739,10 +6864,10 @@
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>116.0</v>
+        <v>63.0</v>
       </c>
       <c r="F17" t="n">
-        <v>51.0</v>
+        <v>33.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -6768,19 +6893,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>20.0</v>
+        <v>29.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>160.0</v>
+        <v>173.0</v>
       </c>
       <c r="F18" t="n">
-        <v>18.0</v>
+        <v>25.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -6806,7 +6931,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
@@ -6815,13 +6940,13 @@
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>148.0</v>
+        <v>183.0</v>
       </c>
       <c r="F19" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="G19" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H19" t="n">
         <v>3.4</v>
@@ -6844,7 +6969,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>33.0</v>
+        <v>46.0</v>
       </c>
       <c r="C20" t="n">
         <v>1.0</v>
@@ -6853,13 +6978,13 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>209.0</v>
+        <v>216.0</v>
       </c>
       <c r="F20" t="n">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="G20" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H20" t="n">
         <v>3.6</v>
@@ -6882,19 +7007,19 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>29.0</v>
+        <v>39.0</v>
       </c>
       <c r="C21" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>147.0</v>
+        <v>156.0</v>
       </c>
       <c r="F21" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="G21" t="n">
         <v>3.0</v>
@@ -6920,19 +7045,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>22.0</v>
+        <v>29.0</v>
       </c>
       <c r="C22" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>230.0</v>
+        <v>316.0</v>
       </c>
       <c r="F22" t="n">
-        <v>150.0</v>
+        <v>139.0</v>
       </c>
       <c r="G22" t="n">
         <v>1.0</v>
@@ -6949,22 +7074,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>165.0</v>
+        <v>168.0</v>
       </c>
       <c r="F23" t="n">
-        <v>21.0</v>
+        <v>15.0</v>
       </c>
       <c r="G23" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H23" t="n">
         <v>3.6</v>
@@ -6978,22 +7103,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>14.0</v>
+        <v>19.0</v>
       </c>
       <c r="C24" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>127.0</v>
+        <v>69.0</v>
       </c>
       <c r="F24" t="n">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="G24" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -7007,22 +7132,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>147.0</v>
+        <v>210.0</v>
       </c>
       <c r="F25" t="n">
-        <v>19.0</v>
+        <v>13.0</v>
       </c>
       <c r="G25" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H25" t="n">
         <v>3.4</v>
@@ -7039,19 +7164,19 @@
         <v>7.0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>75.0</v>
+        <v>99.0</v>
       </c>
       <c r="F26" t="n">
-        <v>7.0</v>
+        <v>20.0</v>
       </c>
       <c r="G26" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H26" t="n">
         <v>3.35</v>
@@ -7065,7 +7190,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>23.0</v>
+        <v>29.0</v>
       </c>
       <c r="C27" t="n">
         <v>4.0</v>
@@ -7074,13 +7199,13 @@
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>297.0</v>
+        <v>89.0</v>
       </c>
       <c r="F27" t="n">
-        <v>193.0</v>
+        <v>37.0</v>
       </c>
       <c r="G27" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H27" t="n">
         <v>3.15</v>
@@ -7094,22 +7219,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>244.0</v>
+        <v>482.0</v>
       </c>
       <c r="F28" t="n">
-        <v>20.0</v>
+        <v>76.0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -7123,22 +7248,22 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>27.0</v>
+        <v>35.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>152.0</v>
+        <v>153.0</v>
       </c>
       <c r="F29" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H29" t="n">
         <v>3.6</v>
@@ -7152,19 +7277,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>284.0</v>
+        <v>156.0</v>
       </c>
       <c r="F30" t="n">
-        <v>36.0</v>
+        <v>15.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -7181,22 +7306,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>202.0</v>
+        <v>179.0</v>
       </c>
       <c r="F31" t="n">
-        <v>104.0</v>
+        <v>73.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>
@@ -7307,19 +7432,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>23.0</v>
+        <v>32.0</v>
       </c>
       <c r="C2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>143.0</v>
+        <v>153.0</v>
       </c>
       <c r="F2" t="n">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -7334,13 +7459,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="M2" t="n">
-        <v>23.0</v>
+        <v>29.0</v>
       </c>
       <c r="N2" t="s">
-        <v>365</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3">
@@ -7348,19 +7473,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>199.0</v>
+        <v>156.0</v>
       </c>
       <c r="F3" t="n">
-        <v>60.0</v>
+        <v>17.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -7386,7 +7511,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>34.0</v>
+        <v>39.0</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -7395,10 +7520,10 @@
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>143.0</v>
+        <v>142.0</v>
       </c>
       <c r="F4" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -7424,19 +7549,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>142.0</v>
+        <v>211.0</v>
       </c>
       <c r="F5" t="n">
-        <v>63.0</v>
+        <v>132.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -7462,19 +7587,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>48.0</v>
+        <v>51.0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>151.0</v>
+        <v>156.0</v>
       </c>
       <c r="F6" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -7500,19 +7625,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>171.0</v>
+        <v>141.0</v>
       </c>
       <c r="F7" t="n">
-        <v>42.0</v>
+        <v>12.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -7538,7 +7663,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="C8" t="n">
         <v>3.0</v>
@@ -7547,10 +7672,10 @@
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>206.0</v>
+        <v>237.0</v>
       </c>
       <c r="F8" t="n">
-        <v>127.0</v>
+        <v>158.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -7576,7 +7701,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="C9" t="n">
         <v>1.0</v>
@@ -7585,10 +7710,10 @@
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>122.0</v>
+        <v>109.0</v>
       </c>
       <c r="F9" t="n">
-        <v>43.0</v>
+        <v>30.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -7614,19 +7739,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>38.0</v>
+        <v>42.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>141.0</v>
+        <v>143.0</v>
       </c>
       <c r="F10" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -7652,19 +7777,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>49.0</v>
+        <v>52.0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>236.0</v>
+        <v>170.0</v>
       </c>
       <c r="F11" t="n">
-        <v>97.0</v>
+        <v>31.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -7690,7 +7815,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>25.0</v>
+        <v>34.0</v>
       </c>
       <c r="C12" t="n">
         <v>1.0</v>
@@ -7699,10 +7824,10 @@
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>142.0</v>
+        <v>189.0</v>
       </c>
       <c r="F12" t="n">
-        <v>14.0</v>
+        <v>61.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -7728,19 +7853,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>52.0</v>
+        <v>54.0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>152.0</v>
+        <v>161.0</v>
       </c>
       <c r="F13" t="n">
-        <v>12.0</v>
+        <v>21.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -7766,7 +7891,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>39.0</v>
+        <v>42.0</v>
       </c>
       <c r="C14" t="n">
         <v>0.0</v>
@@ -7775,10 +7900,10 @@
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>142.0</v>
+        <v>147.0</v>
       </c>
       <c r="F14" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -7804,19 +7929,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>85.0</v>
+        <v>120.0</v>
       </c>
       <c r="F15" t="n">
-        <v>20.0</v>
+        <v>55.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -7842,7 +7967,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>40.0</v>
+        <v>43.0</v>
       </c>
       <c r="C16" t="n">
         <v>0.0</v>
@@ -7880,7 +8005,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="C17" t="n">
         <v>0.0</v>
@@ -7889,10 +8014,10 @@
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>36.0</v>
+        <v>51.0</v>
       </c>
       <c r="F17" t="n">
-        <v>6.0</v>
+        <v>21.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -7918,7 +8043,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>53.0</v>
+        <v>55.0</v>
       </c>
       <c r="C18" t="n">
         <v>1.0</v>
@@ -7927,10 +8052,10 @@
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>194.0</v>
+        <v>159.0</v>
       </c>
       <c r="F18" t="n">
-        <v>52.0</v>
+        <v>17.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -7956,7 +8081,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>41.0</v>
+        <v>44.0</v>
       </c>
       <c r="C19" t="n">
         <v>0.0</v>
@@ -7965,10 +8090,10 @@
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>142.0</v>
+        <v>146.0</v>
       </c>
       <c r="F19" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -7985,7 +8110,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>56.0</v>
+        <v>58.0</v>
       </c>
       <c r="C20" t="n">
         <v>1.0</v>
@@ -7994,10 +8119,10 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>155.0</v>
+        <v>159.0</v>
       </c>
       <c r="F20" t="n">
-        <v>44.0</v>
+        <v>48.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -8014,19 +8139,19 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>42.0</v>
+        <v>45.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>143.0</v>
+        <v>144.0</v>
       </c>
       <c r="F21" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -8043,7 +8168,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="C22" t="n">
         <v>2.0</v>
@@ -8052,10 +8177,10 @@
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>184.0</v>
+        <v>137.0</v>
       </c>
       <c r="F22" t="n">
-        <v>98.0</v>
+        <v>51.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -8072,19 +8197,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>56.0</v>
+        <v>59.0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>151.0</v>
+        <v>168.0</v>
       </c>
       <c r="F23" t="n">
-        <v>12.0</v>
+        <v>29.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -8101,19 +8226,19 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>27.0</v>
+        <v>36.0</v>
       </c>
       <c r="C24" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>157.0</v>
+        <v>130.0</v>
       </c>
       <c r="F24" t="n">
-        <v>41.0</v>
+        <v>14.0</v>
       </c>
       <c r="G24" t="n">
         <v>0.0</v>
@@ -8130,19 +8255,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>162.0</v>
+        <v>141.0</v>
       </c>
       <c r="F25" t="n">
-        <v>33.0</v>
+        <v>12.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -8159,19 +8284,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>30.0</v>
+        <v>37.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>163.0</v>
+        <v>91.0</v>
       </c>
       <c r="F26" t="n">
-        <v>95.0</v>
+        <v>23.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -8188,10 +8313,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>18.0</v>
+        <v>25.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
@@ -8217,7 +8342,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>32.0</v>
+        <v>37.0</v>
       </c>
       <c r="C28" t="n">
         <v>1.0</v>
@@ -8226,10 +8351,10 @@
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>152.0</v>
+        <v>140.0</v>
       </c>
       <c r="F28" t="n">
-        <v>24.0</v>
+        <v>12.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -8246,7 +8371,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>57.0</v>
+        <v>61.0</v>
       </c>
       <c r="C29" t="n">
         <v>1.0</v>
@@ -8255,10 +8380,10 @@
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>195.0</v>
+        <v>152.0</v>
       </c>
       <c r="F29" t="n">
-        <v>55.0</v>
+        <v>12.0</v>
       </c>
       <c r="G29" t="n">
         <v>0.0</v>
@@ -8275,19 +8400,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>44.0</v>
+        <v>46.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>161.0</v>
+        <v>153.0</v>
       </c>
       <c r="F30" t="n">
-        <v>32.0</v>
+        <v>24.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -8304,19 +8429,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>20.0</v>
+        <v>28.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>136.0</v>
+        <v>160.0</v>
       </c>
       <c r="F31" t="n">
-        <v>64.0</v>
+        <v>88.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -8430,19 +8555,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>18.0</v>
+        <v>23.0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>160.0</v>
+        <v>216.0</v>
       </c>
       <c r="F2" t="n">
-        <v>32.0</v>
+        <v>15.0</v>
       </c>
       <c r="G2" t="n">
         <v>3.0</v>
@@ -8457,13 +8582,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>24.0</v>
+        <v>13.0</v>
       </c>
       <c r="M2" t="n">
-        <v>36.0</v>
+        <v>25.0</v>
       </c>
       <c r="N2" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3">
@@ -8471,7 +8596,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>42.0</v>
+        <v>34.0</v>
       </c>
       <c r="C3" t="n">
         <v>3.0</v>
@@ -8480,10 +8605,10 @@
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>160.0</v>
+        <v>151.0</v>
       </c>
       <c r="F3" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="G3" t="n">
         <v>1.0</v>
@@ -8498,13 +8623,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>20.0</v>
+        <v>17.0</v>
       </c>
       <c r="M3" t="n">
-        <v>40.0</v>
+        <v>21.0</v>
       </c>
       <c r="N3" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4">
@@ -8512,22 +8637,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>31.0</v>
+        <v>27.0</v>
       </c>
       <c r="C4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>141.0</v>
+        <v>143.0</v>
       </c>
       <c r="F4" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="G4" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.4</v>
@@ -8542,10 +8667,10 @@
         <v>18.0</v>
       </c>
       <c r="M4" t="n">
-        <v>42.0</v>
+        <v>21.0</v>
       </c>
       <c r="N4" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
     </row>
     <row r="5">
@@ -8553,7 +8678,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -8562,10 +8687,10 @@
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>353.0</v>
+        <v>134.0</v>
       </c>
       <c r="F5" t="n">
-        <v>174.0</v>
+        <v>81.0</v>
       </c>
       <c r="G5" t="n">
         <v>1.0</v>
@@ -8580,13 +8705,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="M5" t="n">
-        <v>48.0</v>
+        <v>25.0</v>
       </c>
       <c r="N5" t="s">
-        <v>360</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6">
@@ -8594,22 +8719,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>42.0</v>
+        <v>35.0</v>
       </c>
       <c r="C6" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>161.0</v>
+        <v>152.0</v>
       </c>
       <c r="F6" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" t="n">
         <v>3.6</v>
@@ -8632,7 +8757,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>30.0</v>
+        <v>27.0</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
@@ -8641,13 +8766,13 @@
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>141.0</v>
+        <v>144.0</v>
       </c>
       <c r="F7" t="n">
-        <v>12.0</v>
+        <v>15.0</v>
       </c>
       <c r="G7" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H7" t="n">
         <v>3.4</v>
@@ -8670,22 +8795,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>42.0</v>
+        <v>378.0</v>
       </c>
       <c r="F8" t="n">
-        <v>25.0</v>
+        <v>154.0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -8708,22 +8833,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="C9" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>174.0</v>
+        <v>220.0</v>
       </c>
       <c r="F9" t="n">
-        <v>87.0</v>
+        <v>112.0</v>
       </c>
       <c r="G9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
         <v>3.15</v>
@@ -8746,22 +8871,22 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>30.0</v>
+        <v>27.0</v>
       </c>
       <c r="C10" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>157.0</v>
+        <v>162.0</v>
       </c>
       <c r="F10" t="n">
-        <v>27.0</v>
+        <v>15.0</v>
       </c>
       <c r="G10" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H10" t="n">
         <v>3.4</v>
@@ -8784,19 +8909,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>48.0</v>
+        <v>34.0</v>
       </c>
       <c r="C11" t="n">
-        <v>11.0</v>
+        <v>2.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>151.0</v>
+        <v>152.0</v>
       </c>
       <c r="F11" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="G11" t="n">
         <v>1.0</v>
@@ -8822,7 +8947,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>24.0</v>
+        <v>22.0</v>
       </c>
       <c r="C12" t="n">
         <v>4.0</v>
@@ -8831,10 +8956,10 @@
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>147.0</v>
+        <v>142.0</v>
       </c>
       <c r="F12" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -8860,22 +8985,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>56.0</v>
+        <v>40.0</v>
       </c>
       <c r="C13" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>231.0</v>
+        <v>223.0</v>
       </c>
       <c r="F13" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="G13" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H13" t="n">
         <v>3.6</v>
@@ -8898,22 +9023,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>36.0</v>
+        <v>28.0</v>
       </c>
       <c r="C14" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>145.0</v>
+        <v>158.0</v>
       </c>
       <c r="F14" t="n">
         <v>16.0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -8936,22 +9061,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>18.0</v>
+        <v>5.0</v>
       </c>
       <c r="C15" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>272.0</v>
+        <v>162.0</v>
       </c>
       <c r="F15" t="n">
-        <v>146.0</v>
+        <v>83.0</v>
       </c>
       <c r="G15" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H15" t="n">
         <v>3.15</v>
@@ -8974,16 +9099,16 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>34.0</v>
+        <v>30.0</v>
       </c>
       <c r="C16" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>132.0</v>
+        <v>136.0</v>
       </c>
       <c r="F16" t="n">
         <v>15.0</v>
@@ -9012,22 +9137,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C17" t="n">
         <v>1.0</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>33.0</v>
+        <v>133.0</v>
       </c>
       <c r="F17" t="n">
-        <v>18.0</v>
+        <v>67.0</v>
       </c>
       <c r="G17" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H17" t="n">
         <v>3.15</v>
@@ -9050,22 +9175,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>49.0</v>
+        <v>33.0</v>
       </c>
       <c r="C18" t="n">
-        <v>11.0</v>
+        <v>7.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>155.0</v>
+        <v>333.0</v>
       </c>
       <c r="F18" t="n">
-        <v>14.0</v>
+        <v>20.0</v>
       </c>
       <c r="G18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H18" t="n">
         <v>3.6</v>
@@ -9088,19 +9213,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>34.0</v>
+        <v>29.0</v>
       </c>
       <c r="C19" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>211.0</v>
+        <v>149.0</v>
       </c>
       <c r="F19" t="n">
-        <v>16.0</v>
+        <v>14.0</v>
       </c>
       <c r="G19" t="n">
         <v>3.0</v>
@@ -9126,19 +9251,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>41.0</v>
+        <v>37.0</v>
       </c>
       <c r="C20" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>129.0</v>
+        <v>191.0</v>
       </c>
       <c r="F20" t="n">
-        <v>12.0</v>
+        <v>19.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -9164,7 +9289,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="C21" t="n">
         <v>2.0</v>
@@ -9173,13 +9298,13 @@
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>160.0</v>
+        <v>155.0</v>
       </c>
       <c r="F21" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="G21" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H21" t="n">
         <v>3.4</v>
@@ -9202,22 +9327,22 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C22" t="n">
         <v>1.0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>43.0</v>
+        <v>123.0</v>
       </c>
       <c r="F22" t="n">
-        <v>15.0</v>
+        <v>45.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H22" t="n">
         <v>3.15</v>
@@ -9231,22 +9356,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>48.0</v>
+        <v>40.0</v>
       </c>
       <c r="C23" t="n">
-        <v>11.0</v>
+        <v>2.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>153.0</v>
+        <v>155.0</v>
       </c>
       <c r="F23" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="G23" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H23" t="n">
         <v>3.6</v>
@@ -9260,7 +9385,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>25.0</v>
+        <v>22.0</v>
       </c>
       <c r="C24" t="n">
         <v>3.0</v>
@@ -9269,13 +9394,13 @@
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>134.0</v>
+        <v>128.0</v>
       </c>
       <c r="F24" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -9289,19 +9414,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>35.0</v>
+        <v>30.0</v>
       </c>
       <c r="C25" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>214.0</v>
+        <v>141.0</v>
       </c>
       <c r="F25" t="n">
-        <v>17.0</v>
+        <v>12.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -9318,10 +9443,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>27.0</v>
+        <v>21.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
@@ -9333,7 +9458,7 @@
         <v>7.0</v>
       </c>
       <c r="G26" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H26" t="n">
         <v>3.35</v>
@@ -9347,19 +9472,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>12.0</v>
+        <v>18.0</v>
       </c>
       <c r="C27" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>244.0</v>
+        <v>267.0</v>
       </c>
       <c r="F27" t="n">
-        <v>130.0</v>
+        <v>127.0</v>
       </c>
       <c r="G27" t="n">
         <v>2.0</v>
@@ -9376,22 +9501,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>26.0</v>
+        <v>22.0</v>
       </c>
       <c r="C28" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>156.0</v>
+        <v>158.0</v>
       </c>
       <c r="F28" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -9405,19 +9530,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>53.0</v>
+        <v>39.0</v>
       </c>
       <c r="C29" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>225.0</v>
+        <v>174.0</v>
       </c>
       <c r="F29" t="n">
-        <v>14.0</v>
+        <v>30.0</v>
       </c>
       <c r="G29" t="n">
         <v>3.0</v>
@@ -9434,22 +9559,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>36.0</v>
+        <v>31.0</v>
       </c>
       <c r="C30" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>142.0</v>
+        <v>150.0</v>
       </c>
       <c r="F30" t="n">
-        <v>13.0</v>
+        <v>21.0</v>
       </c>
       <c r="G30" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H30" t="n">
         <v>3.4</v>
@@ -9466,19 +9591,19 @@
         <v>9.0</v>
       </c>
       <c r="C31" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>221.0</v>
+        <v>226.0</v>
       </c>
       <c r="F31" t="n">
-        <v>115.0</v>
+        <v>116.0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>

</xml_diff>

<commit_message>
All green and good to go (?!)
</commit_message>
<xml_diff>
--- a/Yeezus/output/data.xlsx
+++ b/Yeezus/output/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40028" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42148" uniqueCount="413">
   <si>
     <t>Process ID:</t>
   </si>
@@ -2078,6 +2078,124 @@
   <si>
     <t xml:space="preserve">
 CPU: 0 received 925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 8471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1740
+CPU: 1 received 959
+CPU: 2 received 891
+CPU: 3 received 818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 59720</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1305
+CPU: 1 received 1014
+CPU: 2 received 839
+CPU: 3 received 826</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 28184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 4799
+CPU: 1 received 1064
+CPU: 2 received 702
+CPU: 3 received 641</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 13667</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 12485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1464
+CPU: 1 received 914
+CPU: 2 received 679
+CPU: 3 received 718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 40400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 11241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 996
+CPU: 1 received 699
+CPU: 2 received 695
+CPU: 3 received 645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 55066</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 963
+CPU: 1 received 694
+CPU: 2 received 594
+CPU: 3 received 578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 25311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 3831
+CPU: 1 received 864
+CPU: 2 received 467
+CPU: 3 received 591</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 6626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1343
+CPU: 1 received 907
+CPU: 2 received 1064
+CPU: 3 received 969</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 40843</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 1749
+CPU: 1 received 1370
+CPU: 2 received 1279
+CPU: 3 received 1285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 30269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+CPU: 0 received 2392
+CPU: 1 received 988
+CPU: 2 received 622
+CPU: 3 received 540</t>
   </si>
 </sst>
 </file>
@@ -2195,8 +2313,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="CPU_Table" id="2" insertRow="1" name="CPU_Table" ref="K1:M3" totalsRowCount="1">
-  <autoFilter ref="K1:M3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="CPU_Table" id="2" insertRow="1" name="CPU_Table" ref="K1:M6" totalsRowCount="1">
+  <autoFilter ref="K1:M6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="CPU ID:" totalsRowLabel="Average"/>
     <tableColumn id="2" name="Busy Time (ms):" totalsRowFunction="custom">
@@ -2868,19 +2986,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>19.0</v>
+        <v>115.0</v>
       </c>
       <c r="C2" t="n">
-        <v>10.0</v>
+        <v>63.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>140.0</v>
+        <v>143.0</v>
       </c>
       <c r="F2" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -2895,13 +3013,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>69.0</v>
+        <v>665.0</v>
       </c>
       <c r="M2" t="n">
-        <v>38.0</v>
+        <v>887.0</v>
       </c>
       <c r="N2" t="s">
-        <v>390</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3">
@@ -2909,16 +3027,16 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>31.0</v>
+        <v>207.0</v>
       </c>
       <c r="C3" t="n">
-        <v>5.0</v>
+        <v>32.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>151.0</v>
+        <v>146.0</v>
       </c>
       <c r="F3" t="n">
         <v>12.0</v>
@@ -2947,19 +3065,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>45.0</v>
+        <v>274.0</v>
       </c>
       <c r="C4" t="n">
-        <v>13.0</v>
+        <v>21.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>147.0</v>
+        <v>143.0</v>
       </c>
       <c r="F4" t="n">
-        <v>18.0</v>
+        <v>12.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -2985,19 +3103,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>58.0</v>
+        <v>374.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>38.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>93.0</v>
+        <v>290.0</v>
       </c>
       <c r="F5" t="n">
-        <v>14.0</v>
+        <v>211.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -3023,16 +3141,16 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>62.0</v>
+        <v>416.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>151.0</v>
+        <v>146.0</v>
       </c>
       <c r="F6" t="n">
         <v>12.0</v>
@@ -3061,16 +3179,16 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>63.0</v>
+        <v>427.0</v>
       </c>
       <c r="C7" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>143.0</v>
+        <v>145.0</v>
       </c>
       <c r="F7" t="n">
         <v>14.0</v>
@@ -3099,19 +3217,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>68.0</v>
+        <v>480.0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>146.0</v>
+        <v>109.0</v>
       </c>
       <c r="F8" t="n">
-        <v>67.0</v>
+        <v>30.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -3137,19 +3255,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>71.0</v>
+        <v>641.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>198.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>103.0</v>
+        <v>145.0</v>
       </c>
       <c r="F9" t="n">
-        <v>24.0</v>
+        <v>66.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -3175,19 +3293,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>72.0</v>
+        <v>838.0</v>
       </c>
       <c r="C10" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>146.0</v>
+        <v>150.0</v>
       </c>
       <c r="F10" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -3213,19 +3331,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>75.0</v>
+        <v>857.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>27.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>152.0</v>
+        <v>477.0</v>
       </c>
       <c r="F11" t="n">
-        <v>13.0</v>
+        <v>343.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -3251,19 +3369,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>77.0</v>
+        <v>887.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>140.0</v>
+        <v>165.0</v>
       </c>
       <c r="F12" t="n">
-        <v>12.0</v>
+        <v>36.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -3289,19 +3407,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>78.0</v>
+        <v>898.0</v>
       </c>
       <c r="C13" t="n">
-        <v>2.0</v>
+        <v>26.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>156.0</v>
+        <v>318.0</v>
       </c>
       <c r="F13" t="n">
-        <v>16.0</v>
+        <v>183.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -3327,19 +3445,19 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>81.0</v>
+        <v>927.0</v>
       </c>
       <c r="C14" t="n">
-        <v>2.0</v>
+        <v>35.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>143.0</v>
+        <v>219.0</v>
       </c>
       <c r="F14" t="n">
-        <v>14.0</v>
+        <v>88.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -3365,19 +3483,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>84.0</v>
+        <v>975.0</v>
       </c>
       <c r="C15" t="n">
-        <v>2.0</v>
+        <v>19.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>143.0</v>
+        <v>332.0</v>
       </c>
       <c r="F15" t="n">
-        <v>78.0</v>
+        <v>267.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -3403,19 +3521,19 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>86.0</v>
+        <v>1014.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>128.0</v>
+        <v>205.0</v>
       </c>
       <c r="F16" t="n">
-        <v>11.0</v>
+        <v>86.0</v>
       </c>
       <c r="G16" t="n">
         <v>0.0</v>
@@ -3441,19 +3559,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>87.0</v>
+        <v>1074.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>84.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>43.0</v>
+        <v>1252.0</v>
       </c>
       <c r="F17" t="n">
-        <v>13.0</v>
+        <v>1222.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -3479,19 +3597,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>89.0</v>
+        <v>1163.0</v>
       </c>
       <c r="C18" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>162.0</v>
+        <v>349.0</v>
       </c>
       <c r="F18" t="n">
-        <v>20.0</v>
+        <v>212.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -3517,19 +3635,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>92.0</v>
+        <v>1178.0</v>
       </c>
       <c r="C19" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>141.0</v>
+        <v>196.0</v>
       </c>
       <c r="F19" t="n">
-        <v>12.0</v>
+        <v>65.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -3546,19 +3664,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>95.0</v>
+        <v>1187.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>124.0</v>
+        <v>203.0</v>
       </c>
       <c r="F20" t="n">
-        <v>13.0</v>
+        <v>96.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -3575,19 +3693,19 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>96.0</v>
+        <v>1195.0</v>
       </c>
       <c r="C21" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>141.0</v>
+        <v>153.0</v>
       </c>
       <c r="F21" t="n">
-        <v>12.0</v>
+        <v>22.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -3604,19 +3722,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>99.0</v>
+        <v>1269.0</v>
       </c>
       <c r="C22" t="n">
-        <v>3.0</v>
+        <v>118.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>168.0</v>
+        <v>2297.0</v>
       </c>
       <c r="F22" t="n">
-        <v>82.0</v>
+        <v>2211.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -3633,19 +3751,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>103.0</v>
+        <v>1384.0</v>
       </c>
       <c r="C23" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>160.0</v>
+        <v>151.0</v>
       </c>
       <c r="F23" t="n">
-        <v>21.0</v>
+        <v>17.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -3662,16 +3780,16 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>105.0</v>
+        <v>1391.0</v>
       </c>
       <c r="C24" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>130.0</v>
+        <v>131.0</v>
       </c>
       <c r="F24" t="n">
         <v>14.0</v>
@@ -3691,7 +3809,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>106.0</v>
+        <v>1395.0</v>
       </c>
       <c r="C25" t="n">
         <v>2.0</v>
@@ -3700,10 +3818,10 @@
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>142.0</v>
+        <v>151.0</v>
       </c>
       <c r="F25" t="n">
-        <v>13.0</v>
+        <v>20.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -3720,19 +3838,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>108.0</v>
+        <v>1409.0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>82.0</v>
+        <v>79.0</v>
       </c>
       <c r="F26" t="n">
-        <v>14.0</v>
+        <v>10.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -3749,19 +3867,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>109.0</v>
+        <v>1448.0</v>
       </c>
       <c r="C27" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>123.0</v>
+        <v>103.0</v>
       </c>
       <c r="F27" t="n">
-        <v>72.0</v>
+        <v>52.0</v>
       </c>
       <c r="G27" t="n">
         <v>0.0</v>
@@ -3778,19 +3896,19 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>112.0</v>
+        <v>1453.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>143.0</v>
+        <v>147.0</v>
       </c>
       <c r="F28" t="n">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -3807,19 +3925,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>113.0</v>
+        <v>1460.0</v>
       </c>
       <c r="C29" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>168.0</v>
+        <v>148.0</v>
       </c>
       <c r="F29" t="n">
-        <v>28.0</v>
+        <v>13.0</v>
       </c>
       <c r="G29" t="n">
         <v>0.0</v>
@@ -3836,19 +3954,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>115.0</v>
+        <v>1471.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>142.0</v>
+        <v>143.0</v>
       </c>
       <c r="F30" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -3865,19 +3983,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>117.0</v>
+        <v>1544.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>90.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>116.0</v>
+        <v>1116.0</v>
       </c>
       <c r="F31" t="n">
-        <v>44.0</v>
+        <v>1044.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -3991,22 +4109,22 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.0</v>
+        <v>50.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>102.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>207.0</v>
+        <v>171.0</v>
       </c>
       <c r="F2" t="n">
-        <v>28.0</v>
+        <v>24.0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H2" t="n">
         <v>3.35</v>
@@ -4018,13 +4136,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>23.0</v>
+        <v>105.0</v>
       </c>
       <c r="M2" t="n">
-        <v>29.0</v>
+        <v>272.0</v>
       </c>
       <c r="N2" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3">
@@ -4032,19 +4150,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0</v>
+        <v>49.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>102.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>170.0</v>
+        <v>269.0</v>
       </c>
       <c r="F3" t="n">
-        <v>16.0</v>
+        <v>26.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -4059,13 +4177,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>17.0</v>
+        <v>112.0</v>
       </c>
       <c r="M3" t="n">
-        <v>35.0</v>
+        <v>265.0</v>
       </c>
       <c r="N3" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4">
@@ -4073,22 +4191,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>56.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>98.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>150.0</v>
+        <v>143.0</v>
       </c>
       <c r="F4" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G4" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.4</v>
@@ -4100,13 +4218,13 @@
         <v>2.0</v>
       </c>
       <c r="L4" t="n">
-        <v>15.0</v>
+        <v>84.0</v>
       </c>
       <c r="M4" t="n">
-        <v>37.0</v>
+        <v>292.0</v>
       </c>
       <c r="N4" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5">
@@ -4114,19 +4232,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.0</v>
+        <v>73.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1.0</v>
+        <v>91.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>85.0</v>
+        <v>376.0</v>
       </c>
       <c r="F5" t="n">
-        <v>40.0</v>
+        <v>251.0</v>
       </c>
       <c r="G5" t="n">
         <v>3.0</v>
@@ -4141,13 +4259,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>10.0</v>
+        <v>80.0</v>
       </c>
       <c r="M5" t="n">
-        <v>43.0</v>
+        <v>297.0</v>
       </c>
       <c r="N5" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6">
@@ -4155,16 +4273,16 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>5.0</v>
+        <v>148.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>21.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>166.0</v>
+        <v>240.0</v>
       </c>
       <c r="F6" t="n">
         <v>15.0</v>
@@ -4193,22 +4311,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
+        <v>168.0</v>
+      </c>
+      <c r="C7" t="n">
         <v>7.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>173.0</v>
+        <v>200.0</v>
       </c>
       <c r="F7" t="n">
-        <v>20.0</v>
+        <v>12.0</v>
       </c>
       <c r="G7" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
         <v>3.4</v>
@@ -4231,22 +4349,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>8.0</v>
+        <v>170.0</v>
       </c>
       <c r="C8" t="n">
-        <v>5.0</v>
+        <v>12.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>258.0</v>
+        <v>182.0</v>
       </c>
       <c r="F8" t="n">
-        <v>107.0</v>
+        <v>146.0</v>
       </c>
       <c r="G8" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -4269,19 +4387,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>10.0</v>
+        <v>173.0</v>
       </c>
       <c r="C9" t="n">
-        <v>4.0</v>
+        <v>19.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>151.0</v>
+        <v>542.0</v>
       </c>
       <c r="F9" t="n">
-        <v>64.0</v>
+        <v>318.0</v>
       </c>
       <c r="G9" t="n">
         <v>3.0</v>
@@ -4307,19 +4425,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>11.0</v>
+        <v>192.0</v>
       </c>
       <c r="C10" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>151.0</v>
+        <v>305.0</v>
       </c>
       <c r="F10" t="n">
-        <v>22.0</v>
+        <v>32.0</v>
       </c>
       <c r="G10" t="n">
         <v>3.0</v>
@@ -4345,22 +4463,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>14.0</v>
+        <v>193.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>151.0</v>
+        <v>170.0</v>
       </c>
       <c r="F11" t="n">
-        <v>12.0</v>
+        <v>25.0</v>
       </c>
       <c r="G11" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" t="n">
         <v>3.6</v>
@@ -4383,22 +4501,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>15.0</v>
+        <v>193.0</v>
       </c>
       <c r="C12" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>177.0</v>
+        <v>176.0</v>
       </c>
       <c r="F12" t="n">
-        <v>20.0</v>
+        <v>18.0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H12" t="n">
         <v>3.35</v>
@@ -4421,22 +4539,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>15.0</v>
+        <v>195.0</v>
       </c>
       <c r="C13" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>185.0</v>
+        <v>211.0</v>
       </c>
       <c r="F13" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
       <c r="G13" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H13" t="n">
         <v>3.6</v>
@@ -4459,22 +4577,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>15.0</v>
+        <v>196.0</v>
       </c>
       <c r="C14" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>142.0</v>
+        <v>144.0</v>
       </c>
       <c r="F14" t="n">
         <v>13.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -4497,22 +4615,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>18.0</v>
+        <v>201.0</v>
       </c>
       <c r="C15" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>133.0</v>
+        <v>201.0</v>
       </c>
       <c r="F15" t="n">
-        <v>70.0</v>
+        <v>84.0</v>
       </c>
       <c r="G15" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H15" t="n">
         <v>3.15</v>
@@ -4535,22 +4653,22 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>20.0</v>
+        <v>204.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>128.0</v>
+        <v>106.0</v>
       </c>
       <c r="F16" t="n">
         <v>11.0</v>
       </c>
       <c r="G16" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H16" t="n">
         <v>3.4</v>
@@ -4573,22 +4691,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>20.0</v>
+        <v>207.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>85.0</v>
+        <v>76.0</v>
       </c>
       <c r="F17" t="n">
-        <v>42.0</v>
+        <v>29.0</v>
       </c>
       <c r="G17" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H17" t="n">
         <v>3.15</v>
@@ -4611,19 +4729,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>21.0</v>
+        <v>210.0</v>
       </c>
       <c r="C18" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>161.0</v>
+        <v>154.0</v>
       </c>
       <c r="F18" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="G18" t="n">
         <v>2.0</v>
@@ -4649,22 +4767,22 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>21.0</v>
+        <v>210.0</v>
       </c>
       <c r="C19" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>327.0</v>
+        <v>161.0</v>
       </c>
       <c r="F19" t="n">
-        <v>31.0</v>
+        <v>19.0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H19" t="n">
         <v>3.4</v>
@@ -4687,19 +4805,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>24.0</v>
+        <v>210.0</v>
       </c>
       <c r="C20" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>209.0</v>
+        <v>119.0</v>
       </c>
       <c r="F20" t="n">
-        <v>28.0</v>
+        <v>12.0</v>
       </c>
       <c r="G20" t="n">
         <v>3.0</v>
@@ -4725,22 +4843,22 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>26.0</v>
+        <v>211.0</v>
       </c>
       <c r="C21" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>238.0</v>
+        <v>250.0</v>
       </c>
       <c r="F21" t="n">
-        <v>49.0</v>
+        <v>26.0</v>
       </c>
       <c r="G21" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H21" t="n">
         <v>3.4</v>
@@ -4763,19 +4881,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>27.0</v>
+        <v>215.0</v>
       </c>
       <c r="C22" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>338.0</v>
+        <v>476.0</v>
       </c>
       <c r="F22" t="n">
-        <v>252.0</v>
+        <v>244.0</v>
       </c>
       <c r="G22" t="n">
         <v>1.0</v>
@@ -4792,22 +4910,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>33.0</v>
+        <v>225.0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>191.0</v>
+        <v>406.0</v>
       </c>
       <c r="F23" t="n">
-        <v>37.0</v>
+        <v>58.0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H23" t="n">
         <v>3.6</v>
@@ -4821,7 +4939,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>34.0</v>
+        <v>228.0</v>
       </c>
       <c r="C24" t="n">
         <v>2.0</v>
@@ -4830,13 +4948,13 @@
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>260.0</v>
+        <v>128.0</v>
       </c>
       <c r="F24" t="n">
-        <v>43.0</v>
+        <v>11.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -4850,22 +4968,22 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>35.0</v>
+        <v>229.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>223.0</v>
+        <v>173.0</v>
       </c>
       <c r="F25" t="n">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="G25" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H25" t="n">
         <v>3.4</v>
@@ -4879,22 +4997,22 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>36.0</v>
+        <v>230.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>95.0</v>
+        <v>78.0</v>
       </c>
       <c r="F26" t="n">
         <v>9.0</v>
       </c>
       <c r="G26" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H26" t="n">
         <v>3.35</v>
@@ -4908,19 +5026,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>38.0</v>
+        <v>232.0</v>
       </c>
       <c r="C27" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>205.0</v>
+        <v>140.0</v>
       </c>
       <c r="F27" t="n">
-        <v>134.0</v>
+        <v>64.0</v>
       </c>
       <c r="G27" t="n">
         <v>2.0</v>
@@ -4937,22 +5055,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>41.0</v>
+        <v>240.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>28.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>230.0</v>
+        <v>205.0</v>
       </c>
       <c r="F28" t="n">
-        <v>29.0</v>
+        <v>24.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -4966,19 +5084,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>42.0</v>
+        <v>262.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>107.0</v>
+        <v>503.0</v>
       </c>
       <c r="F29" t="n">
-        <v>10.0</v>
+        <v>56.0</v>
       </c>
       <c r="G29" t="n">
         <v>3.0</v>
@@ -4995,22 +5113,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>43.0</v>
+        <v>249.0</v>
       </c>
       <c r="C30" t="n">
-        <v>6.0</v>
+        <v>56.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>355.0</v>
+        <v>176.0</v>
       </c>
       <c r="F30" t="n">
-        <v>32.0</v>
+        <v>16.0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H30" t="n">
         <v>3.4</v>
@@ -5024,22 +5142,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>50.0</v>
+        <v>295.0</v>
       </c>
       <c r="C31" t="n">
-        <v>4.0</v>
+        <v>123.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>318.0</v>
+        <v>2679.0</v>
       </c>
       <c r="F31" t="n">
-        <v>191.0</v>
+        <v>2502.0</v>
       </c>
       <c r="G31" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>
@@ -5150,19 +5268,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>51.0</v>
+        <v>2159.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>143.0</v>
+        <v>230.0</v>
       </c>
       <c r="F2" t="n">
-        <v>15.0</v>
+        <v>101.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -5177,13 +5295,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>47.0</v>
+        <v>808.0</v>
       </c>
       <c r="M2" t="n">
-        <v>16.0</v>
+        <v>1299.0</v>
       </c>
       <c r="N2" t="s">
-        <v>386</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3">
@@ -5191,19 +5309,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>33.0</v>
+        <v>1361.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>172.0</v>
+        <v>147.0</v>
       </c>
       <c r="F3" t="n">
-        <v>33.0</v>
+        <v>13.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -5229,19 +5347,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>20.0</v>
+        <v>915.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>143.0</v>
+        <v>174.0</v>
       </c>
       <c r="F4" t="n">
-        <v>14.0</v>
+        <v>43.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -5267,19 +5385,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>24.0</v>
+        <v>1164.0</v>
       </c>
       <c r="C5" t="n">
-        <v>2.0</v>
+        <v>194.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>137.0</v>
+        <v>5957.0</v>
       </c>
       <c r="F5" t="n">
-        <v>58.0</v>
+        <v>5878.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -5305,19 +5423,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>45.0</v>
+        <v>2095.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>161.0</v>
+        <v>305.0</v>
       </c>
       <c r="F6" t="n">
-        <v>22.0</v>
+        <v>171.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -5343,19 +5461,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>18.0</v>
+        <v>905.0</v>
       </c>
       <c r="C7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>158.0</v>
+        <v>152.0</v>
       </c>
       <c r="F7" t="n">
-        <v>29.0</v>
+        <v>21.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -5381,19 +5499,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>27.0</v>
+        <v>1111.0</v>
       </c>
       <c r="C8" t="n">
-        <v>2.0</v>
+        <v>116.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>166.0</v>
+        <v>3686.0</v>
       </c>
       <c r="F8" t="n">
-        <v>87.0</v>
+        <v>3607.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -5419,19 +5537,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1.0</v>
+        <v>264.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>177.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>145.0</v>
+        <v>2299.0</v>
       </c>
       <c r="F9" t="n">
-        <v>66.0</v>
+        <v>2220.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -5457,19 +5575,19 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>52.0</v>
+        <v>2158.0</v>
       </c>
       <c r="C10" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>167.0</v>
+        <v>225.0</v>
       </c>
       <c r="F10" t="n">
-        <v>38.0</v>
+        <v>94.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -5495,19 +5613,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>8.0</v>
+        <v>572.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>153.0</v>
+        <v>194.0</v>
       </c>
       <c r="F11" t="n">
-        <v>14.0</v>
+        <v>60.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -5533,19 +5651,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>45.0</v>
+        <v>2112.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>40.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>140.0</v>
+        <v>1624.0</v>
       </c>
       <c r="F12" t="n">
-        <v>12.0</v>
+        <v>1495.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -5571,19 +5689,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>11.0</v>
+        <v>618.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>16.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>160.0</v>
+        <v>368.0</v>
       </c>
       <c r="F13" t="n">
-        <v>20.0</v>
+        <v>233.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -5609,19 +5727,19 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>3.0</v>
+        <v>457.0</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0</v>
+        <v>21.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>141.0</v>
+        <v>184.0</v>
       </c>
       <c r="F14" t="n">
-        <v>12.0</v>
+        <v>53.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -5647,19 +5765,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>55.0</v>
+        <v>2186.0</v>
       </c>
       <c r="C15" t="n">
-        <v>6.0</v>
+        <v>63.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>100.0</v>
+        <v>2992.0</v>
       </c>
       <c r="F15" t="n">
-        <v>35.0</v>
+        <v>2927.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -5685,19 +5803,19 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>26.0</v>
+        <v>1229.0</v>
       </c>
       <c r="C16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>129.0</v>
+        <v>151.0</v>
       </c>
       <c r="F16" t="n">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
       <c r="G16" t="n">
         <v>0.0</v>
@@ -5723,19 +5841,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>15.0</v>
+        <v>804.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>34.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>46.0</v>
+        <v>844.0</v>
       </c>
       <c r="F17" t="n">
-        <v>16.0</v>
+        <v>814.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -5761,19 +5879,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>33.0</v>
+        <v>1436.0</v>
       </c>
       <c r="C18" t="n">
-        <v>2.0</v>
+        <v>45.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>181.0</v>
+        <v>1998.0</v>
       </c>
       <c r="F18" t="n">
-        <v>39.0</v>
+        <v>1861.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -5799,19 +5917,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>4.0</v>
+        <v>489.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>49.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>142.0</v>
+        <v>488.0</v>
       </c>
       <c r="F19" t="n">
-        <v>13.0</v>
+        <v>357.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -5828,19 +5946,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>63.0</v>
+        <v>2255.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>132.0</v>
+        <v>296.0</v>
       </c>
       <c r="F20" t="n">
-        <v>21.0</v>
+        <v>189.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -5857,19 +5975,19 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>59.0</v>
+        <v>2162.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>143.0</v>
+        <v>153.0</v>
       </c>
       <c r="F21" t="n">
-        <v>14.0</v>
+        <v>22.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -5886,19 +6004,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>38.0</v>
+        <v>1812.0</v>
       </c>
       <c r="C22" t="n">
-        <v>4.0</v>
+        <v>242.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>162.0</v>
+        <v>8635.0</v>
       </c>
       <c r="F22" t="n">
-        <v>76.0</v>
+        <v>8549.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -5915,19 +6033,19 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>8.0</v>
+        <v>570.0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>151.0</v>
+        <v>193.0</v>
       </c>
       <c r="F23" t="n">
-        <v>12.0</v>
+        <v>59.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -5944,19 +6062,19 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>28.0</v>
+        <v>1233.0</v>
       </c>
       <c r="C24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>127.0</v>
+        <v>147.0</v>
       </c>
       <c r="F24" t="n">
-        <v>11.0</v>
+        <v>30.0</v>
       </c>
       <c r="G24" t="n">
         <v>0.0</v>
@@ -5973,19 +6091,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>18.0</v>
+        <v>903.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>150.0</v>
+        <v>191.0</v>
       </c>
       <c r="F25" t="n">
-        <v>21.0</v>
+        <v>60.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -6002,19 +6120,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>11.0</v>
+        <v>602.0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>76.0</v>
+        <v>304.0</v>
       </c>
       <c r="F26" t="n">
-        <v>8.0</v>
+        <v>235.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -6031,19 +6149,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>37.0</v>
+        <v>1864.0</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0</v>
+        <v>216.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>100.0</v>
+        <v>7446.0</v>
       </c>
       <c r="F27" t="n">
-        <v>49.0</v>
+        <v>7395.0</v>
       </c>
       <c r="G27" t="n">
         <v>0.0</v>
@@ -6060,19 +6178,19 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>12.0</v>
+        <v>662.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>81.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>164.0</v>
+        <v>2106.0</v>
       </c>
       <c r="F28" t="n">
-        <v>36.0</v>
+        <v>1977.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -6089,19 +6207,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>46.0</v>
+        <v>2101.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>152.0</v>
+        <v>211.0</v>
       </c>
       <c r="F29" t="n">
-        <v>12.0</v>
+        <v>76.0</v>
       </c>
       <c r="G29" t="n">
         <v>0.0</v>
@@ -6118,19 +6236,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>63.0</v>
+        <v>2254.0</v>
       </c>
       <c r="C30" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>164.0</v>
+        <v>355.0</v>
       </c>
       <c r="F30" t="n">
-        <v>35.0</v>
+        <v>224.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -6147,19 +6265,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>15.0</v>
+        <v>819.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>78.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>108.0</v>
+        <v>1914.0</v>
       </c>
       <c r="F31" t="n">
-        <v>36.0</v>
+        <v>1842.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -6273,7 +6391,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>44.0</v>
+        <v>347.0</v>
       </c>
       <c r="C2" t="n">
         <v>2.0</v>
@@ -6282,13 +6400,13 @@
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>156.0</v>
+        <v>160.0</v>
       </c>
       <c r="F2" t="n">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="G2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H2" t="n">
         <v>3.35</v>
@@ -6300,13 +6418,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>22.0</v>
+        <v>93.0</v>
       </c>
       <c r="M2" t="n">
-        <v>25.0</v>
+        <v>243.0</v>
       </c>
       <c r="N2" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3">
@@ -6314,7 +6432,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>29.0</v>
+        <v>322.0</v>
       </c>
       <c r="C3" t="n">
         <v>2.0</v>
@@ -6323,13 +6441,13 @@
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>158.0</v>
+        <v>153.0</v>
       </c>
       <c r="F3" t="n">
-        <v>19.0</v>
+        <v>13.0</v>
       </c>
       <c r="G3" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n">
         <v>3.6</v>
@@ -6341,13 +6459,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>22.0</v>
+        <v>42.0</v>
       </c>
       <c r="M3" t="n">
-        <v>25.0</v>
+        <v>264.0</v>
       </c>
       <c r="N3" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
     </row>
     <row r="4">
@@ -6355,22 +6473,22 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>17.0</v>
+        <v>297.0</v>
       </c>
       <c r="C4" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>194.0</v>
+        <v>241.0</v>
       </c>
       <c r="F4" t="n">
-        <v>13.0</v>
+        <v>18.0</v>
       </c>
       <c r="G4" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" t="n">
         <v>3.4</v>
@@ -6382,13 +6500,13 @@
         <v>2.0</v>
       </c>
       <c r="L4" t="n">
-        <v>11.0</v>
+        <v>36.0</v>
       </c>
       <c r="M4" t="n">
-        <v>36.0</v>
+        <v>271.0</v>
       </c>
       <c r="N4" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5">
@@ -6396,22 +6514,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>22.0</v>
+        <v>311.0</v>
       </c>
       <c r="C5" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>329.0</v>
+        <v>374.0</v>
       </c>
       <c r="F5" t="n">
-        <v>129.0</v>
+        <v>259.0</v>
       </c>
       <c r="G5" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H5" t="n">
         <v>3.15</v>
@@ -6423,13 +6541,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>10.0</v>
+        <v>31.0</v>
       </c>
       <c r="M5" t="n">
-        <v>37.0</v>
+        <v>276.0</v>
       </c>
       <c r="N5" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6">
@@ -6437,7 +6555,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>36.0</v>
+        <v>343.0</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -6446,10 +6564,10 @@
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>156.0</v>
+        <v>167.0</v>
       </c>
       <c r="F6" t="n">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="G6" t="n">
         <v>2.0</v>
@@ -6475,22 +6593,22 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>16.0</v>
+        <v>295.0</v>
       </c>
       <c r="C7" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>148.0</v>
+        <v>179.0</v>
       </c>
       <c r="F7" t="n">
-        <v>13.0</v>
+        <v>19.0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H7" t="n">
         <v>3.4</v>
@@ -6513,22 +6631,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>22.0</v>
+        <v>307.0</v>
       </c>
       <c r="C8" t="n">
-        <v>4.0</v>
+        <v>12.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>123.0</v>
+        <v>527.0</v>
       </c>
       <c r="F8" t="n">
-        <v>66.0</v>
+        <v>367.0</v>
       </c>
       <c r="G8" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -6551,22 +6669,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0</v>
+        <v>87.0</v>
       </c>
       <c r="C9" t="n">
-        <v>2.0</v>
+        <v>182.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>273.0</v>
+        <v>3287.0</v>
       </c>
       <c r="F9" t="n">
-        <v>130.0</v>
+        <v>3134.0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H9" t="n">
         <v>3.15</v>
@@ -6589,7 +6707,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>44.0</v>
+        <v>347.0</v>
       </c>
       <c r="C10" t="n">
         <v>2.0</v>
@@ -6598,10 +6716,10 @@
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>157.0</v>
+        <v>136.0</v>
       </c>
       <c r="F10" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="G10" t="n">
         <v>1.0</v>
@@ -6627,22 +6745,22 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>5.0</v>
+        <v>254.0</v>
       </c>
       <c r="C11" t="n">
-        <v>2.0</v>
+        <v>24.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>277.0</v>
+        <v>146.0</v>
       </c>
       <c r="F11" t="n">
-        <v>24.0</v>
+        <v>12.0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H11" t="n">
         <v>3.6</v>
@@ -6665,22 +6783,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>36.0</v>
+        <v>342.0</v>
       </c>
       <c r="C12" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>262.0</v>
+        <v>159.0</v>
       </c>
       <c r="F12" t="n">
-        <v>22.0</v>
+        <v>16.0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H12" t="n">
         <v>3.35</v>
@@ -6703,22 +6821,22 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>8.0</v>
+        <v>277.0</v>
       </c>
       <c r="C13" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>276.0</v>
+        <v>285.0</v>
       </c>
       <c r="F13" t="n">
-        <v>51.0</v>
+        <v>23.0</v>
       </c>
       <c r="G13" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n">
         <v>3.6</v>
@@ -6741,22 +6859,22 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>4.0</v>
+        <v>219.0</v>
       </c>
       <c r="C14" t="n">
-        <v>1.0</v>
+        <v>56.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>219.0</v>
+        <v>151.0</v>
       </c>
       <c r="F14" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
       <c r="G14" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -6779,19 +6897,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>41.0</v>
+        <v>350.0</v>
       </c>
       <c r="C15" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>486.0</v>
+        <v>610.0</v>
       </c>
       <c r="F15" t="n">
-        <v>261.0</v>
+        <v>400.0</v>
       </c>
       <c r="G15" t="n">
         <v>2.0</v>
@@ -6817,7 +6935,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>20.0</v>
+        <v>301.0</v>
       </c>
       <c r="C16" t="n">
         <v>2.0</v>
@@ -6826,13 +6944,13 @@
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>128.0</v>
+        <v>120.0</v>
       </c>
       <c r="F16" t="n">
-        <v>11.0</v>
+        <v>25.0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H16" t="n">
         <v>3.4</v>
@@ -6855,22 +6973,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>13.0</v>
+        <v>284.0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>63.0</v>
+        <v>201.0</v>
       </c>
       <c r="F17" t="n">
-        <v>33.0</v>
+        <v>168.0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H17" t="n">
         <v>3.15</v>
@@ -6893,7 +7011,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>29.0</v>
+        <v>321.0</v>
       </c>
       <c r="C18" t="n">
         <v>2.0</v>
@@ -6902,13 +7020,13 @@
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>173.0</v>
+        <v>163.0</v>
       </c>
       <c r="F18" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H18" t="n">
         <v>3.6</v>
@@ -6931,19 +7049,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>3.0</v>
+        <v>219.0</v>
       </c>
       <c r="C19" t="n">
-        <v>1.0</v>
+        <v>56.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>183.0</v>
+        <v>164.0</v>
       </c>
       <c r="F19" t="n">
-        <v>18.0</v>
+        <v>15.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -6969,22 +7087,22 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>46.0</v>
+        <v>362.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>216.0</v>
+        <v>207.0</v>
       </c>
       <c r="F20" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="G20" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H20" t="n">
         <v>3.6</v>
@@ -7007,10 +7125,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>39.0</v>
+        <v>346.0</v>
       </c>
       <c r="C21" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
@@ -7019,7 +7137,7 @@
         <v>156.0</v>
       </c>
       <c r="F21" t="n">
-        <v>23.0</v>
+        <v>20.0</v>
       </c>
       <c r="G21" t="n">
         <v>3.0</v>
@@ -7045,22 +7163,22 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>29.0</v>
+        <v>324.0</v>
       </c>
       <c r="C22" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>316.0</v>
+        <v>453.0</v>
       </c>
       <c r="F22" t="n">
-        <v>139.0</v>
+        <v>328.0</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H22" t="n">
         <v>3.15</v>
@@ -7074,22 +7192,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>5.0</v>
+        <v>263.0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>168.0</v>
+        <v>153.0</v>
       </c>
       <c r="F23" t="n">
-        <v>15.0</v>
+        <v>13.0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H23" t="n">
         <v>3.6</v>
@@ -7103,22 +7221,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>19.0</v>
+        <v>299.0</v>
       </c>
       <c r="C24" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>69.0</v>
+        <v>144.0</v>
       </c>
       <c r="F24" t="n">
-        <v>9.0</v>
+        <v>27.0</v>
       </c>
       <c r="G24" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -7132,7 +7250,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>15.0</v>
+        <v>293.0</v>
       </c>
       <c r="C25" t="n">
         <v>3.0</v>
@@ -7141,10 +7259,10 @@
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>210.0</v>
+        <v>176.0</v>
       </c>
       <c r="F25" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="G25" t="n">
         <v>3.0</v>
@@ -7161,19 +7279,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>7.0</v>
+        <v>268.0</v>
       </c>
       <c r="C26" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>99.0</v>
+        <v>82.0</v>
       </c>
       <c r="F26" t="n">
-        <v>20.0</v>
+        <v>9.0</v>
       </c>
       <c r="G26" t="n">
         <v>3.0</v>
@@ -7190,22 +7308,22 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>29.0</v>
+        <v>333.0</v>
       </c>
       <c r="C27" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>89.0</v>
+        <v>254.0</v>
       </c>
       <c r="F27" t="n">
-        <v>37.0</v>
+        <v>182.0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H27" t="n">
         <v>3.15</v>
@@ -7219,22 +7337,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>8.0</v>
+        <v>267.0</v>
       </c>
       <c r="C28" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>482.0</v>
+        <v>149.0</v>
       </c>
       <c r="F28" t="n">
-        <v>76.0</v>
+        <v>20.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -7248,7 +7366,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>35.0</v>
+        <v>341.0</v>
       </c>
       <c r="C29" t="n">
         <v>2.0</v>
@@ -7257,13 +7375,13 @@
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>153.0</v>
+        <v>161.0</v>
       </c>
       <c r="F29" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="G29" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H29" t="n">
         <v>3.6</v>
@@ -7277,7 +7395,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>46.0</v>
+        <v>362.0</v>
       </c>
       <c r="C30" t="n">
         <v>2.0</v>
@@ -7286,13 +7404,13 @@
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>156.0</v>
+        <v>293.0</v>
       </c>
       <c r="F30" t="n">
-        <v>15.0</v>
+        <v>35.0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H30" t="n">
         <v>3.4</v>
@@ -7306,22 +7424,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>12.0</v>
+        <v>283.0</v>
       </c>
       <c r="C31" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>179.0</v>
+        <v>281.0</v>
       </c>
       <c r="F31" t="n">
-        <v>73.0</v>
+        <v>173.0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>
@@ -7432,19 +7550,19 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>32.0</v>
+        <v>1060.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>153.0</v>
+        <v>395.0</v>
       </c>
       <c r="F2" t="n">
-        <v>25.0</v>
+        <v>266.0</v>
       </c>
       <c r="G2" t="n">
         <v>0.0</v>
@@ -7459,13 +7577,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>33.0</v>
+        <v>449.0</v>
       </c>
       <c r="M2" t="n">
-        <v>29.0</v>
+        <v>984.0</v>
       </c>
       <c r="N2" t="s">
-        <v>388</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3">
@@ -7473,19 +7591,19 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>49.0</v>
+        <v>1377.0</v>
       </c>
       <c r="C3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="D3">
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>156.0</v>
+        <v>147.0</v>
       </c>
       <c r="F3" t="n">
-        <v>17.0</v>
+        <v>13.0</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -7511,19 +7629,19 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>39.0</v>
+        <v>1126.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="D4">
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>142.0</v>
+        <v>228.0</v>
       </c>
       <c r="F4" t="n">
-        <v>13.0</v>
+        <v>97.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -7549,19 +7667,19 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0</v>
+        <v>145.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>135.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>211.0</v>
+        <v>1785.0</v>
       </c>
       <c r="F5" t="n">
-        <v>132.0</v>
+        <v>1706.0</v>
       </c>
       <c r="G5" t="n">
         <v>0.0</v>
@@ -7587,19 +7705,19 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>51.0</v>
+        <v>1386.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0</v>
+        <v>25.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>156.0</v>
+        <v>768.0</v>
       </c>
       <c r="F6" t="n">
-        <v>17.0</v>
+        <v>634.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -7625,19 +7743,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>40.0</v>
+        <v>1137.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>141.0</v>
+        <v>901.0</v>
       </c>
       <c r="F7" t="n">
-        <v>12.0</v>
+        <v>770.0</v>
       </c>
       <c r="G7" t="n">
         <v>0.0</v>
@@ -7663,19 +7781,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>2.0</v>
+        <v>215.0</v>
       </c>
       <c r="C8" t="n">
-        <v>3.0</v>
+        <v>73.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>237.0</v>
+        <v>521.0</v>
       </c>
       <c r="F8" t="n">
-        <v>158.0</v>
+        <v>442.0</v>
       </c>
       <c r="G8" t="n">
         <v>0.0</v>
@@ -7701,19 +7819,19 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>13.0</v>
+        <v>326.0</v>
       </c>
       <c r="C9" t="n">
-        <v>1.0</v>
+        <v>87.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>109.0</v>
+        <v>2919.0</v>
       </c>
       <c r="F9" t="n">
-        <v>30.0</v>
+        <v>2840.0</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -7739,10 +7857,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>42.0</v>
+        <v>1162.0</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D10">
         <f>$B$10+$C$10</f>
@@ -7751,7 +7869,7 @@
         <v>143.0</v>
       </c>
       <c r="F10" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -7777,19 +7895,19 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>52.0</v>
+        <v>1415.0</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D11">
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>170.0</v>
+        <v>190.0</v>
       </c>
       <c r="F11" t="n">
-        <v>31.0</v>
+        <v>56.0</v>
       </c>
       <c r="G11" t="n">
         <v>0.0</v>
@@ -7815,19 +7933,19 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>34.0</v>
+        <v>1072.0</v>
       </c>
       <c r="C12" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>189.0</v>
+        <v>324.0</v>
       </c>
       <c r="F12" t="n">
-        <v>61.0</v>
+        <v>195.0</v>
       </c>
       <c r="G12" t="n">
         <v>0.0</v>
@@ -7853,19 +7971,19 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>54.0</v>
+        <v>1415.0</v>
       </c>
       <c r="C13" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="D13">
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>161.0</v>
+        <v>353.0</v>
       </c>
       <c r="F13" t="n">
-        <v>21.0</v>
+        <v>218.0</v>
       </c>
       <c r="G13" t="n">
         <v>0.0</v>
@@ -7891,19 +8009,19 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>42.0</v>
+        <v>1165.0</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="D14">
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>147.0</v>
+        <v>235.0</v>
       </c>
       <c r="F14" t="n">
-        <v>18.0</v>
+        <v>104.0</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -7929,19 +8047,19 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>16.0</v>
+        <v>449.0</v>
       </c>
       <c r="C15" t="n">
-        <v>7.0</v>
+        <v>103.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>120.0</v>
+        <v>4484.0</v>
       </c>
       <c r="F15" t="n">
-        <v>55.0</v>
+        <v>4419.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -7967,19 +8085,19 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>43.0</v>
+        <v>1172.0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="D16">
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>128.0</v>
+        <v>216.0</v>
       </c>
       <c r="F16" t="n">
-        <v>11.0</v>
+        <v>97.0</v>
       </c>
       <c r="G16" t="n">
         <v>0.0</v>
@@ -8005,19 +8123,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>21.0</v>
+        <v>568.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>36.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>51.0</v>
+        <v>1382.0</v>
       </c>
       <c r="F17" t="n">
-        <v>21.0</v>
+        <v>1352.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -8043,19 +8161,19 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>55.0</v>
+        <v>1427.0</v>
       </c>
       <c r="C18" t="n">
-        <v>1.0</v>
+        <v>13.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>159.0</v>
+        <v>705.0</v>
       </c>
       <c r="F18" t="n">
-        <v>17.0</v>
+        <v>568.0</v>
       </c>
       <c r="G18" t="n">
         <v>0.0</v>
@@ -8081,19 +8199,19 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>44.0</v>
+        <v>1180.0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>146.0</v>
+        <v>475.0</v>
       </c>
       <c r="F19" t="n">
-        <v>17.0</v>
+        <v>344.0</v>
       </c>
       <c r="G19" t="n">
         <v>0.0</v>
@@ -8110,19 +8228,19 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>58.0</v>
+        <v>1441.0</v>
       </c>
       <c r="C20" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D20">
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>159.0</v>
+        <v>167.0</v>
       </c>
       <c r="F20" t="n">
-        <v>48.0</v>
+        <v>60.0</v>
       </c>
       <c r="G20" t="n">
         <v>0.0</v>
@@ -8139,19 +8257,19 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>45.0</v>
+        <v>1195.0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D21">
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>144.0</v>
+        <v>231.0</v>
       </c>
       <c r="F21" t="n">
-        <v>15.0</v>
+        <v>100.0</v>
       </c>
       <c r="G21" t="n">
         <v>0.0</v>
@@ -8168,19 +8286,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>23.0</v>
+        <v>656.0</v>
       </c>
       <c r="C22" t="n">
-        <v>2.0</v>
+        <v>130.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>137.0</v>
+        <v>4954.0</v>
       </c>
       <c r="F22" t="n">
-        <v>51.0</v>
+        <v>4868.0</v>
       </c>
       <c r="G22" t="n">
         <v>0.0</v>
@@ -8197,7 +8315,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>59.0</v>
+        <v>1444.0</v>
       </c>
       <c r="C23" t="n">
         <v>1.0</v>
@@ -8206,10 +8324,10 @@
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>168.0</v>
+        <v>162.0</v>
       </c>
       <c r="F23" t="n">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="G23" t="n">
         <v>0.0</v>
@@ -8226,19 +8344,19 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>36.0</v>
+        <v>1081.0</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>130.0</v>
+        <v>338.0</v>
       </c>
       <c r="F24" t="n">
-        <v>14.0</v>
+        <v>221.0</v>
       </c>
       <c r="G24" t="n">
         <v>0.0</v>
@@ -8255,19 +8373,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>46.0</v>
+        <v>1207.0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>141.0</v>
+        <v>1068.0</v>
       </c>
       <c r="F25" t="n">
-        <v>12.0</v>
+        <v>937.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -8284,19 +8402,19 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>37.0</v>
+        <v>1090.0</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="D26">
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>91.0</v>
+        <v>124.0</v>
       </c>
       <c r="F26" t="n">
-        <v>23.0</v>
+        <v>55.0</v>
       </c>
       <c r="G26" t="n">
         <v>0.0</v>
@@ -8313,19 +8431,19 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>25.0</v>
+        <v>813.0</v>
       </c>
       <c r="C27" t="n">
-        <v>2.0</v>
+        <v>76.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>78.0</v>
+        <v>2477.0</v>
       </c>
       <c r="F27" t="n">
-        <v>27.0</v>
+        <v>2426.0</v>
       </c>
       <c r="G27" t="n">
         <v>0.0</v>
@@ -8342,19 +8460,19 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>37.0</v>
+        <v>1099.0</v>
       </c>
       <c r="C28" t="n">
-        <v>1.0</v>
+        <v>22.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>140.0</v>
+        <v>761.0</v>
       </c>
       <c r="F28" t="n">
-        <v>12.0</v>
+        <v>632.0</v>
       </c>
       <c r="G28" t="n">
         <v>0.0</v>
@@ -8371,19 +8489,19 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>61.0</v>
+        <v>1447.0</v>
       </c>
       <c r="C29" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="D29">
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>152.0</v>
+        <v>353.0</v>
       </c>
       <c r="F29" t="n">
-        <v>12.0</v>
+        <v>218.0</v>
       </c>
       <c r="G29" t="n">
         <v>0.0</v>
@@ -8400,19 +8518,19 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>46.0</v>
+        <v>1297.0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0</v>
+        <v>76.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>153.0</v>
+        <v>2601.0</v>
       </c>
       <c r="F30" t="n">
-        <v>24.0</v>
+        <v>2470.0</v>
       </c>
       <c r="G30" t="n">
         <v>0.0</v>
@@ -8429,19 +8547,19 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>28.0</v>
+        <v>937.0</v>
       </c>
       <c r="C31" t="n">
-        <v>3.0</v>
+        <v>118.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>160.0</v>
+        <v>3988.0</v>
       </c>
       <c r="F31" t="n">
-        <v>88.0</v>
+        <v>3916.0</v>
       </c>
       <c r="G31" t="n">
         <v>0.0</v>
@@ -8555,22 +8673,22 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>23.0</v>
+        <v>267.0</v>
       </c>
       <c r="C2" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D2">
         <f>$B$2+$C$2</f>
       </c>
       <c r="E2" t="n">
-        <v>216.0</v>
+        <v>333.0</v>
       </c>
       <c r="F2" t="n">
-        <v>15.0</v>
+        <v>69.0</v>
       </c>
       <c r="G2" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
         <v>3.35</v>
@@ -8582,13 +8700,13 @@
         <v>0.0</v>
       </c>
       <c r="L2" t="n">
-        <v>13.0</v>
+        <v>72.0</v>
       </c>
       <c r="M2" t="n">
-        <v>25.0</v>
+        <v>212.0</v>
       </c>
       <c r="N2" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
     </row>
     <row r="3">
@@ -8596,7 +8714,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>34.0</v>
+        <v>292.0</v>
       </c>
       <c r="C3" t="n">
         <v>3.0</v>
@@ -8605,13 +8723,13 @@
         <f>$B$3+$C$3</f>
       </c>
       <c r="E3" t="n">
-        <v>151.0</v>
+        <v>189.0</v>
       </c>
       <c r="F3" t="n">
-        <v>13.0</v>
+        <v>19.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n">
         <v>3.6</v>
@@ -8623,13 +8741,13 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="n">
-        <v>17.0</v>
+        <v>30.0</v>
       </c>
       <c r="M3" t="n">
-        <v>21.0</v>
+        <v>252.0</v>
       </c>
       <c r="N3" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4">
@@ -8637,7 +8755,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>27.0</v>
+        <v>271.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -8646,10 +8764,10 @@
         <f>$B$4+$C$4</f>
       </c>
       <c r="E4" t="n">
-        <v>143.0</v>
+        <v>156.0</v>
       </c>
       <c r="F4" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="G4" t="n">
         <v>0.0</v>
@@ -8664,13 +8782,13 @@
         <v>2.0</v>
       </c>
       <c r="L4" t="n">
-        <v>18.0</v>
+        <v>22.0</v>
       </c>
       <c r="M4" t="n">
-        <v>21.0</v>
+        <v>259.0</v>
       </c>
       <c r="N4" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5">
@@ -8678,22 +8796,22 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>4.0</v>
+        <v>118.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>37.0</v>
       </c>
       <c r="D5">
         <f>$B$5+$C$5</f>
       </c>
       <c r="E5" t="n">
-        <v>134.0</v>
+        <v>594.0</v>
       </c>
       <c r="F5" t="n">
-        <v>81.0</v>
+        <v>391.0</v>
       </c>
       <c r="G5" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H5" t="n">
         <v>3.15</v>
@@ -8705,13 +8823,13 @@
         <v>3.0</v>
       </c>
       <c r="L5" t="n">
-        <v>14.0</v>
+        <v>17.0</v>
       </c>
       <c r="M5" t="n">
-        <v>25.0</v>
+        <v>264.0</v>
       </c>
       <c r="N5" t="s">
-        <v>389</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6">
@@ -8719,22 +8837,22 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>35.0</v>
+        <v>288.0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D6">
         <f>$B$6+$C$6</f>
       </c>
       <c r="E6" t="n">
-        <v>152.0</v>
+        <v>155.0</v>
       </c>
       <c r="F6" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="G6" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H6" t="n">
         <v>3.6</v>
@@ -8757,19 +8875,19 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>27.0</v>
+        <v>274.0</v>
       </c>
       <c r="C7" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="D7">
         <f>$B$7+$C$7</f>
       </c>
       <c r="E7" t="n">
-        <v>144.0</v>
+        <v>383.0</v>
       </c>
       <c r="F7" t="n">
-        <v>15.0</v>
+        <v>142.0</v>
       </c>
       <c r="G7" t="n">
         <v>3.0</v>
@@ -8795,22 +8913,22 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>13.0</v>
+        <v>189.0</v>
       </c>
       <c r="C8" t="n">
-        <v>7.0</v>
+        <v>45.0</v>
       </c>
       <c r="D8">
         <f>$B$8+$C$8</f>
       </c>
       <c r="E8" t="n">
-        <v>378.0</v>
+        <v>1213.0</v>
       </c>
       <c r="F8" t="n">
-        <v>154.0</v>
+        <v>1040.0</v>
       </c>
       <c r="G8" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" t="n">
         <v>3.15</v>
@@ -8833,22 +8951,22 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>10.0</v>
+        <v>197.0</v>
       </c>
       <c r="C9" t="n">
-        <v>5.0</v>
+        <v>56.0</v>
       </c>
       <c r="D9">
         <f>$B$9+$C$9</f>
       </c>
       <c r="E9" t="n">
-        <v>220.0</v>
+        <v>537.0</v>
       </c>
       <c r="F9" t="n">
-        <v>112.0</v>
+        <v>407.0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H9" t="n">
         <v>3.15</v>
@@ -8871,7 +8989,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>27.0</v>
+        <v>280.0</v>
       </c>
       <c r="C10" t="n">
         <v>2.0</v>
@@ -8880,13 +8998,13 @@
         <f>$B$10+$C$10</f>
       </c>
       <c r="E10" t="n">
-        <v>162.0</v>
+        <v>157.0</v>
       </c>
       <c r="F10" t="n">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="G10" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H10" t="n">
         <v>3.4</v>
@@ -8909,7 +9027,7 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="n">
-        <v>34.0</v>
+        <v>286.0</v>
       </c>
       <c r="C11" t="n">
         <v>2.0</v>
@@ -8918,13 +9036,13 @@
         <f>$B$11+$C$11</f>
       </c>
       <c r="E11" t="n">
-        <v>152.0</v>
+        <v>227.0</v>
       </c>
       <c r="F11" t="n">
-        <v>13.0</v>
+        <v>23.0</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="n">
         <v>3.6</v>
@@ -8947,22 +9065,22 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>22.0</v>
+        <v>264.0</v>
       </c>
       <c r="C12" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D12">
         <f>$B$12+$C$12</f>
       </c>
       <c r="E12" t="n">
-        <v>142.0</v>
+        <v>141.0</v>
       </c>
       <c r="F12" t="n">
-        <v>14.0</v>
+        <v>12.0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H12" t="n">
         <v>3.35</v>
@@ -8985,7 +9103,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>40.0</v>
+        <v>288.0</v>
       </c>
       <c r="C13" t="n">
         <v>2.0</v>
@@ -8994,13 +9112,13 @@
         <f>$B$13+$C$13</f>
       </c>
       <c r="E13" t="n">
-        <v>223.0</v>
+        <v>228.0</v>
       </c>
       <c r="F13" t="n">
-        <v>21.0</v>
+        <v>14.0</v>
       </c>
       <c r="G13" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n">
         <v>3.6</v>
@@ -9023,7 +9141,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>28.0</v>
+        <v>271.0</v>
       </c>
       <c r="C14" t="n">
         <v>1.0</v>
@@ -9032,13 +9150,13 @@
         <f>$B$14+$C$14</f>
       </c>
       <c r="E14" t="n">
-        <v>158.0</v>
+        <v>147.0</v>
       </c>
       <c r="F14" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="G14" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
         <v>3.4</v>
@@ -9061,22 +9179,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>5.0</v>
+        <v>200.0</v>
       </c>
       <c r="C15" t="n">
-        <v>3.0</v>
+        <v>62.0</v>
       </c>
       <c r="D15">
         <f>$B$15+$C$15</f>
       </c>
       <c r="E15" t="n">
-        <v>162.0</v>
+        <v>509.0</v>
       </c>
       <c r="F15" t="n">
-        <v>83.0</v>
+        <v>330.0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H15" t="n">
         <v>3.15</v>
@@ -9099,7 +9217,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>30.0</v>
+        <v>270.0</v>
       </c>
       <c r="C16" t="n">
         <v>1.0</v>
@@ -9108,10 +9226,10 @@
         <f>$B$16+$C$16</f>
       </c>
       <c r="E16" t="n">
-        <v>136.0</v>
+        <v>98.0</v>
       </c>
       <c r="F16" t="n">
-        <v>15.0</v>
+        <v>9.0</v>
       </c>
       <c r="G16" t="n">
         <v>3.0</v>
@@ -9137,19 +9255,19 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>4.0</v>
+        <v>92.0</v>
       </c>
       <c r="C17" t="n">
-        <v>1.0</v>
+        <v>54.0</v>
       </c>
       <c r="D17">
         <f>$B$17+$C$17</f>
       </c>
       <c r="E17" t="n">
-        <v>133.0</v>
+        <v>141.0</v>
       </c>
       <c r="F17" t="n">
-        <v>67.0</v>
+        <v>57.0</v>
       </c>
       <c r="G17" t="n">
         <v>0.0</v>
@@ -9175,22 +9293,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>33.0</v>
+        <v>291.0</v>
       </c>
       <c r="C18" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="D18">
         <f>$B$18+$C$18</f>
       </c>
       <c r="E18" t="n">
-        <v>333.0</v>
+        <v>190.0</v>
       </c>
       <c r="F18" t="n">
-        <v>20.0</v>
+        <v>17.0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H18" t="n">
         <v>3.6</v>
@@ -9213,22 +9331,22 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>29.0</v>
+        <v>280.0</v>
       </c>
       <c r="C19" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D19">
         <f>$B$19+$C$19</f>
       </c>
       <c r="E19" t="n">
-        <v>149.0</v>
+        <v>368.0</v>
       </c>
       <c r="F19" t="n">
-        <v>14.0</v>
+        <v>47.0</v>
       </c>
       <c r="G19" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H19" t="n">
         <v>3.4</v>
@@ -9251,7 +9369,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>37.0</v>
+        <v>285.0</v>
       </c>
       <c r="C20" t="n">
         <v>2.0</v>
@@ -9260,13 +9378,13 @@
         <f>$B$20+$C$20</f>
       </c>
       <c r="E20" t="n">
-        <v>191.0</v>
+        <v>201.0</v>
       </c>
       <c r="F20" t="n">
-        <v>19.0</v>
+        <v>39.0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H20" t="n">
         <v>3.6</v>
@@ -9289,7 +9407,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>30.0</v>
+        <v>270.0</v>
       </c>
       <c r="C21" t="n">
         <v>2.0</v>
@@ -9298,13 +9416,13 @@
         <f>$B$21+$C$21</f>
       </c>
       <c r="E21" t="n">
-        <v>155.0</v>
+        <v>151.0</v>
       </c>
       <c r="F21" t="n">
         <v>14.0</v>
       </c>
       <c r="G21" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H21" t="n">
         <v>3.4</v>
@@ -9327,19 +9445,19 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>19.0</v>
+        <v>79.0</v>
       </c>
       <c r="C22" t="n">
-        <v>1.0</v>
+        <v>65.0</v>
       </c>
       <c r="D22">
         <f>$B$22+$C$22</f>
       </c>
       <c r="E22" t="n">
-        <v>123.0</v>
+        <v>904.0</v>
       </c>
       <c r="F22" t="n">
-        <v>45.0</v>
+        <v>716.0</v>
       </c>
       <c r="G22" t="n">
         <v>3.0</v>
@@ -9356,22 +9474,22 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>40.0</v>
+        <v>291.0</v>
       </c>
       <c r="C23" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="D23">
         <f>$B$23+$C$23</f>
       </c>
       <c r="E23" t="n">
-        <v>155.0</v>
+        <v>625.0</v>
       </c>
       <c r="F23" t="n">
-        <v>16.0</v>
+        <v>107.0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H23" t="n">
         <v>3.6</v>
@@ -9385,22 +9503,22 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>22.0</v>
+        <v>266.0</v>
       </c>
       <c r="C24" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D24">
         <f>$B$24+$C$24</f>
       </c>
       <c r="E24" t="n">
-        <v>128.0</v>
+        <v>151.0</v>
       </c>
       <c r="F24" t="n">
-        <v>12.0</v>
+        <v>35.0</v>
       </c>
       <c r="G24" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H24" t="n">
         <v>3.35</v>
@@ -9414,19 +9532,19 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>30.0</v>
+        <v>279.0</v>
       </c>
       <c r="C25" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D25">
         <f>$B$25+$C$25</f>
       </c>
       <c r="E25" t="n">
-        <v>141.0</v>
+        <v>179.0</v>
       </c>
       <c r="F25" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="G25" t="n">
         <v>0.0</v>
@@ -9443,7 +9561,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>21.0</v>
+        <v>263.0</v>
       </c>
       <c r="C26" t="n">
         <v>2.0</v>
@@ -9452,13 +9570,13 @@
         <f>$B$26+$C$26</f>
       </c>
       <c r="E26" t="n">
-        <v>75.0</v>
+        <v>123.0</v>
       </c>
       <c r="F26" t="n">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H26" t="n">
         <v>3.35</v>
@@ -9472,22 +9590,22 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>18.0</v>
+        <v>221.0</v>
       </c>
       <c r="C27" t="n">
-        <v>3.0</v>
+        <v>23.0</v>
       </c>
       <c r="D27">
         <f>$B$27+$C$27</f>
       </c>
       <c r="E27" t="n">
-        <v>267.0</v>
+        <v>151.0</v>
       </c>
       <c r="F27" t="n">
-        <v>127.0</v>
+        <v>113.0</v>
       </c>
       <c r="G27" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H27" t="n">
         <v>3.15</v>
@@ -9501,22 +9619,22 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>22.0</v>
+        <v>263.0</v>
       </c>
       <c r="C28" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="D28">
         <f>$B$28+$C$28</f>
       </c>
       <c r="E28" t="n">
-        <v>158.0</v>
+        <v>161.0</v>
       </c>
       <c r="F28" t="n">
-        <v>24.0</v>
+        <v>15.0</v>
       </c>
       <c r="G28" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H28" t="n">
         <v>3.35</v>
@@ -9530,7 +9648,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>39.0</v>
+        <v>286.0</v>
       </c>
       <c r="C29" t="n">
         <v>2.0</v>
@@ -9539,13 +9657,13 @@
         <f>$B$29+$C$29</f>
       </c>
       <c r="E29" t="n">
-        <v>174.0</v>
+        <v>156.0</v>
       </c>
       <c r="F29" t="n">
-        <v>30.0</v>
+        <v>14.0</v>
       </c>
       <c r="G29" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="H29" t="n">
         <v>3.6</v>
@@ -9559,22 +9677,22 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>31.0</v>
+        <v>280.0</v>
       </c>
       <c r="C30" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D30">
         <f>$B$30+$C$30</f>
       </c>
       <c r="E30" t="n">
-        <v>150.0</v>
+        <v>181.0</v>
       </c>
       <c r="F30" t="n">
-        <v>21.0</v>
+        <v>38.0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H30" t="n">
         <v>3.4</v>
@@ -9588,22 +9706,22 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>9.0</v>
+        <v>113.0</v>
       </c>
       <c r="C31" t="n">
-        <v>1.0</v>
+        <v>60.0</v>
       </c>
       <c r="D31">
         <f>$B$31+$C$31</f>
       </c>
       <c r="E31" t="n">
-        <v>226.0</v>
+        <v>694.0</v>
       </c>
       <c r="F31" t="n">
-        <v>116.0</v>
+        <v>494.0</v>
       </c>
       <c r="G31" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H31" t="n">
         <v>3.15</v>

</xml_diff>